<commit_message>
Valores parciales y acumulados para EV3
</commit_message>
<xml_diff>
--- a/Planificación del proyecto/EV2, EV3 Equipo 01.xlsx
+++ b/Planificación del proyecto/EV2, EV3 Equipo 01.xlsx
@@ -1513,7 +1513,7 @@
     <xf numFmtId="9" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="166">
+  <cellXfs count="165">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="165" fontId="3" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1726,32 +1726,14 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="46" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1780,75 +1762,43 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="44" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="20" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="21" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="22" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="11" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
@@ -1880,6 +1830,33 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
@@ -1889,6 +1866,42 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="20" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="21" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="22" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="23" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="23" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -1897,20 +1910,6 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="23" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="23" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="46" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -3342,59 +3341,59 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:22" x14ac:dyDescent="0.2">
-      <c r="A1" s="110" t="s">
+      <c r="A1" s="104" t="s">
         <v>4</v>
       </c>
-      <c r="B1" s="112" t="s">
+      <c r="B1" s="106" t="s">
         <v>5</v>
       </c>
-      <c r="C1" s="113"/>
-      <c r="D1" s="110" t="s">
+      <c r="C1" s="107"/>
+      <c r="D1" s="104" t="s">
         <v>6</v>
       </c>
-      <c r="E1" s="116" t="s">
+      <c r="E1" s="110" t="s">
         <v>7</v>
       </c>
-      <c r="F1" s="116" t="s">
+      <c r="F1" s="110" t="s">
         <v>8</v>
       </c>
-      <c r="G1" s="116" t="s">
+      <c r="G1" s="110" t="s">
         <v>9</v>
       </c>
-      <c r="H1" s="102" t="s">
+      <c r="H1" s="112" t="s">
         <v>10</v>
       </c>
-      <c r="I1" s="103"/>
-      <c r="J1" s="104"/>
-      <c r="K1" s="105" t="s">
+      <c r="I1" s="113"/>
+      <c r="J1" s="114"/>
+      <c r="K1" s="115" t="s">
         <v>11</v>
       </c>
-      <c r="L1" s="103"/>
-      <c r="M1" s="104"/>
-      <c r="N1" s="102" t="s">
-        <v>0</v>
-      </c>
-      <c r="O1" s="103"/>
-      <c r="P1" s="104"/>
-      <c r="Q1" s="105" t="s">
+      <c r="L1" s="113"/>
+      <c r="M1" s="114"/>
+      <c r="N1" s="112" t="s">
+        <v>0</v>
+      </c>
+      <c r="O1" s="113"/>
+      <c r="P1" s="114"/>
+      <c r="Q1" s="115" t="s">
         <v>1</v>
       </c>
-      <c r="R1" s="103"/>
-      <c r="S1" s="104"/>
-      <c r="T1" s="102" t="s">
+      <c r="R1" s="113"/>
+      <c r="S1" s="114"/>
+      <c r="T1" s="112" t="s">
         <v>20</v>
       </c>
-      <c r="U1" s="103"/>
-      <c r="V1" s="104"/>
+      <c r="U1" s="113"/>
+      <c r="V1" s="114"/>
     </row>
     <row r="2" spans="1:22" x14ac:dyDescent="0.2">
-      <c r="A2" s="111"/>
-      <c r="B2" s="114"/>
-      <c r="C2" s="115"/>
-      <c r="D2" s="111"/>
-      <c r="E2" s="117"/>
-      <c r="F2" s="117"/>
-      <c r="G2" s="117"/>
+      <c r="A2" s="105"/>
+      <c r="B2" s="108"/>
+      <c r="C2" s="109"/>
+      <c r="D2" s="105"/>
+      <c r="E2" s="111"/>
+      <c r="F2" s="111"/>
+      <c r="G2" s="111"/>
       <c r="H2" s="2">
         <v>44081</v>
       </c>
@@ -3439,17 +3438,17 @@
       </c>
     </row>
     <row r="3" spans="1:22" x14ac:dyDescent="0.2">
-      <c r="A3" s="111"/>
+      <c r="A3" s="105"/>
       <c r="B3" s="18" t="s">
         <v>2</v>
       </c>
       <c r="C3" s="18" t="s">
         <v>3</v>
       </c>
-      <c r="D3" s="111"/>
-      <c r="E3" s="117"/>
-      <c r="F3" s="117"/>
-      <c r="G3" s="117"/>
+      <c r="D3" s="105"/>
+      <c r="E3" s="111"/>
+      <c r="F3" s="111"/>
+      <c r="G3" s="111"/>
       <c r="H3" s="19" t="s">
         <v>12</v>
       </c>
@@ -4915,13 +4914,13 @@
       <c r="D36" s="39"/>
       <c r="E36" s="26"/>
       <c r="F36" s="37"/>
-      <c r="G36" s="97"/>
-      <c r="H36" s="97"/>
-      <c r="I36" s="97"/>
-      <c r="J36" s="97"/>
-      <c r="K36" s="97"/>
-      <c r="L36" s="97"/>
-      <c r="M36" s="97"/>
+      <c r="G36" s="116"/>
+      <c r="H36" s="116"/>
+      <c r="I36" s="116"/>
+      <c r="J36" s="116"/>
+      <c r="K36" s="116"/>
+      <c r="L36" s="116"/>
+      <c r="M36" s="116"/>
       <c r="N36" s="37"/>
       <c r="O36" s="37"/>
       <c r="P36" s="37"/>
@@ -4966,58 +4965,58 @@
       <c r="G38" s="24"/>
     </row>
     <row r="39" spans="1:22" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="106"/>
-      <c r="B39" s="106"/>
-      <c r="C39" s="106"/>
-      <c r="D39" s="106"/>
-      <c r="E39" s="106"/>
+      <c r="A39" s="100"/>
+      <c r="B39" s="100"/>
+      <c r="C39" s="100"/>
+      <c r="D39" s="100"/>
+      <c r="E39" s="100"/>
       <c r="F39" s="24"/>
-      <c r="G39" s="107" t="s">
+      <c r="G39" s="101" t="s">
         <v>114</v>
       </c>
-      <c r="H39" s="108"/>
-      <c r="I39" s="108"/>
-      <c r="J39" s="108"/>
-      <c r="K39" s="108"/>
-      <c r="L39" s="108"/>
-      <c r="M39" s="109"/>
+      <c r="H39" s="102"/>
+      <c r="I39" s="102"/>
+      <c r="J39" s="102"/>
+      <c r="K39" s="102"/>
+      <c r="L39" s="102"/>
+      <c r="M39" s="103"/>
     </row>
     <row r="40" spans="1:22" x14ac:dyDescent="0.2">
-      <c r="A40" s="100"/>
-      <c r="B40" s="101"/>
-      <c r="C40" s="101"/>
-      <c r="D40" s="101"/>
-      <c r="E40" s="101"/>
+      <c r="A40" s="117"/>
+      <c r="B40" s="118"/>
+      <c r="C40" s="118"/>
+      <c r="D40" s="118"/>
+      <c r="E40" s="118"/>
       <c r="F40" s="24"/>
-      <c r="G40" s="97"/>
-      <c r="H40" s="97"/>
-      <c r="I40" s="97"/>
-      <c r="J40" s="97"/>
-      <c r="K40" s="97"/>
-      <c r="L40" s="97"/>
-      <c r="M40" s="97"/>
+      <c r="G40" s="116"/>
+      <c r="H40" s="116"/>
+      <c r="I40" s="116"/>
+      <c r="J40" s="116"/>
+      <c r="K40" s="116"/>
+      <c r="L40" s="116"/>
+      <c r="M40" s="116"/>
     </row>
     <row r="41" spans="1:22" x14ac:dyDescent="0.2">
-      <c r="A41" s="100"/>
-      <c r="B41" s="101"/>
-      <c r="C41" s="101"/>
-      <c r="D41" s="101"/>
-      <c r="E41" s="101"/>
+      <c r="A41" s="117"/>
+      <c r="B41" s="118"/>
+      <c r="C41" s="118"/>
+      <c r="D41" s="118"/>
+      <c r="E41" s="118"/>
       <c r="F41" s="24"/>
-      <c r="G41" s="97"/>
-      <c r="H41" s="97"/>
-      <c r="I41" s="97"/>
-      <c r="J41" s="97"/>
-      <c r="K41" s="97"/>
-      <c r="L41" s="97"/>
-      <c r="M41" s="97"/>
+      <c r="G41" s="116"/>
+      <c r="H41" s="116"/>
+      <c r="I41" s="116"/>
+      <c r="J41" s="116"/>
+      <c r="K41" s="116"/>
+      <c r="L41" s="116"/>
+      <c r="M41" s="116"/>
     </row>
     <row r="42" spans="1:22" x14ac:dyDescent="0.2">
-      <c r="A42" s="100"/>
-      <c r="B42" s="101"/>
-      <c r="C42" s="101"/>
-      <c r="D42" s="101"/>
-      <c r="E42" s="101"/>
+      <c r="A42" s="117"/>
+      <c r="B42" s="118"/>
+      <c r="C42" s="118"/>
+      <c r="D42" s="118"/>
+      <c r="E42" s="118"/>
       <c r="F42" s="24"/>
       <c r="G42" s="22"/>
       <c r="H42" s="22"/>
@@ -5026,29 +5025,29 @@
       <c r="K42" s="22"/>
     </row>
     <row r="43" spans="1:22" x14ac:dyDescent="0.2">
-      <c r="G43" s="97"/>
-      <c r="H43" s="97"/>
+      <c r="G43" s="116"/>
+      <c r="H43" s="116"/>
       <c r="I43" s="22"/>
       <c r="J43" s="22"/>
       <c r="K43" s="22"/>
     </row>
     <row r="44" spans="1:22" x14ac:dyDescent="0.2">
-      <c r="G44" s="97"/>
-      <c r="H44" s="97"/>
-      <c r="I44" s="97"/>
-      <c r="J44" s="97"/>
-      <c r="K44" s="97"/>
-      <c r="L44" s="97"/>
-      <c r="M44" s="97"/>
+      <c r="G44" s="116"/>
+      <c r="H44" s="116"/>
+      <c r="I44" s="116"/>
+      <c r="J44" s="116"/>
+      <c r="K44" s="116"/>
+      <c r="L44" s="116"/>
+      <c r="M44" s="116"/>
     </row>
     <row r="45" spans="1:22" x14ac:dyDescent="0.2">
-      <c r="G45" s="97"/>
-      <c r="H45" s="97"/>
-      <c r="I45" s="97"/>
-      <c r="J45" s="97"/>
-      <c r="K45" s="97"/>
-      <c r="L45" s="97"/>
-      <c r="M45" s="97"/>
+      <c r="G45" s="116"/>
+      <c r="H45" s="116"/>
+      <c r="I45" s="116"/>
+      <c r="J45" s="116"/>
+      <c r="K45" s="116"/>
+      <c r="L45" s="116"/>
+      <c r="M45" s="116"/>
     </row>
     <row r="47" spans="1:22" x14ac:dyDescent="0.2">
       <c r="D47" s="24"/>
@@ -5068,10 +5067,10 @@
         <f>E56-E54</f>
         <v>0</v>
       </c>
-      <c r="I50" s="94" t="s">
+      <c r="I50" s="96" t="s">
         <v>28</v>
       </c>
-      <c r="J50" s="94"/>
+      <c r="J50" s="96"/>
       <c r="K50" s="98"/>
       <c r="L50" s="99"/>
       <c r="M50" s="99"/>
@@ -5089,10 +5088,10 @@
         <f>E56-E55</f>
         <v>0</v>
       </c>
-      <c r="I51" s="94" t="s">
+      <c r="I51" s="96" t="s">
         <v>29</v>
       </c>
-      <c r="J51" s="94"/>
+      <c r="J51" s="96"/>
       <c r="K51" s="98"/>
       <c r="L51" s="99"/>
       <c r="M51" s="99"/>
@@ -5102,10 +5101,10 @@
       <c r="Q51" s="99"/>
     </row>
     <row r="52" spans="4:19" x14ac:dyDescent="0.2">
-      <c r="D52" s="95" t="s">
+      <c r="D52" s="119" t="s">
         <v>105</v>
       </c>
-      <c r="E52" s="96"/>
+      <c r="E52" s="120"/>
       <c r="G52" s="32" t="s">
         <v>23</v>
       </c>
@@ -5113,10 +5112,10 @@
         <f>E56/E54</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="I52" s="94" t="s">
+      <c r="I52" s="96" t="s">
         <v>31</v>
       </c>
-      <c r="J52" s="94"/>
+      <c r="J52" s="96"/>
       <c r="K52" s="98"/>
       <c r="L52" s="99"/>
       <c r="M52" s="99"/>
@@ -5138,10 +5137,10 @@
         <f>E56/E55</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="I53" s="94" t="s">
+      <c r="I53" s="96" t="s">
         <v>30</v>
       </c>
-      <c r="J53" s="94"/>
+      <c r="J53" s="96"/>
       <c r="K53" s="98"/>
       <c r="L53" s="99"/>
       <c r="M53" s="99"/>
@@ -5165,10 +5164,10 @@
         <f>E53-E56</f>
         <v>0</v>
       </c>
-      <c r="I54" s="94" t="s">
+      <c r="I54" s="96" t="s">
         <v>32</v>
       </c>
-      <c r="J54" s="94"/>
+      <c r="J54" s="96"/>
       <c r="K54" s="98"/>
       <c r="L54" s="99"/>
       <c r="M54" s="99"/>
@@ -5192,10 +5191,10 @@
         <f>(E53-E56)/(H52*H53)</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="I55" s="94" t="s">
+      <c r="I55" s="96" t="s">
         <v>40</v>
       </c>
-      <c r="J55" s="94"/>
+      <c r="J55" s="96"/>
       <c r="K55" s="98"/>
       <c r="L55" s="99"/>
       <c r="M55" s="99"/>
@@ -5219,10 +5218,10 @@
         <f>E55+(E53-E56)</f>
         <v>0</v>
       </c>
-      <c r="I56" s="94" t="s">
+      <c r="I56" s="96" t="s">
         <v>34</v>
       </c>
-      <c r="J56" s="94"/>
+      <c r="J56" s="96"/>
       <c r="K56" s="98"/>
       <c r="L56" s="99"/>
       <c r="M56" s="99"/>
@@ -5242,10 +5241,10 @@
         <f>E53/H53</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="I57" s="94" t="s">
+      <c r="I57" s="96" t="s">
         <v>35</v>
       </c>
-      <c r="J57" s="118"/>
+      <c r="J57" s="97"/>
       <c r="K57" s="98"/>
       <c r="L57" s="99"/>
       <c r="M57" s="99"/>
@@ -5265,10 +5264,10 @@
         <f>E55+(E53-E56)/(H52*H53)</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="I58" s="94" t="s">
+      <c r="I58" s="96" t="s">
         <v>41</v>
       </c>
-      <c r="J58" s="118"/>
+      <c r="J58" s="97"/>
       <c r="K58" s="98"/>
       <c r="L58" s="99"/>
       <c r="M58" s="99"/>
@@ -5289,10 +5288,10 @@
         <f>(E53-E56)/(E53-E55)</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="I59" s="94" t="s">
+      <c r="I59" s="96" t="s">
         <v>42</v>
       </c>
-      <c r="J59" s="118"/>
+      <c r="J59" s="97"/>
       <c r="K59" s="98"/>
       <c r="L59" s="99"/>
       <c r="M59" s="99"/>
@@ -5508,20 +5507,25 @@
     </row>
   </sheetData>
   <mergeCells count="43">
-    <mergeCell ref="I59:J59"/>
-    <mergeCell ref="K59:Q59"/>
-    <mergeCell ref="I56:J56"/>
-    <mergeCell ref="K56:Q56"/>
-    <mergeCell ref="I57:J57"/>
-    <mergeCell ref="K57:Q57"/>
-    <mergeCell ref="I58:J58"/>
-    <mergeCell ref="K58:Q58"/>
-    <mergeCell ref="I53:J53"/>
-    <mergeCell ref="K53:Q53"/>
-    <mergeCell ref="I54:J54"/>
-    <mergeCell ref="K54:Q54"/>
-    <mergeCell ref="I55:J55"/>
-    <mergeCell ref="K55:Q55"/>
+    <mergeCell ref="I50:J50"/>
+    <mergeCell ref="I51:J51"/>
+    <mergeCell ref="I52:J52"/>
+    <mergeCell ref="D52:E52"/>
+    <mergeCell ref="G45:M45"/>
+    <mergeCell ref="K50:Q50"/>
+    <mergeCell ref="K51:Q51"/>
+    <mergeCell ref="K52:Q52"/>
+    <mergeCell ref="A40:E40"/>
+    <mergeCell ref="A41:E41"/>
+    <mergeCell ref="A42:E42"/>
+    <mergeCell ref="G40:M40"/>
+    <mergeCell ref="G41:M41"/>
+    <mergeCell ref="N1:P1"/>
+    <mergeCell ref="Q1:S1"/>
+    <mergeCell ref="T1:V1"/>
+    <mergeCell ref="G43:H43"/>
+    <mergeCell ref="G44:M44"/>
+    <mergeCell ref="G36:M36"/>
     <mergeCell ref="A39:E39"/>
     <mergeCell ref="G39:M39"/>
     <mergeCell ref="A1:A3"/>
@@ -5532,25 +5536,20 @@
     <mergeCell ref="G1:G3"/>
     <mergeCell ref="H1:J1"/>
     <mergeCell ref="K1:M1"/>
-    <mergeCell ref="N1:P1"/>
-    <mergeCell ref="Q1:S1"/>
-    <mergeCell ref="T1:V1"/>
-    <mergeCell ref="G43:H43"/>
-    <mergeCell ref="G44:M44"/>
-    <mergeCell ref="G36:M36"/>
-    <mergeCell ref="A40:E40"/>
-    <mergeCell ref="A41:E41"/>
-    <mergeCell ref="A42:E42"/>
-    <mergeCell ref="G40:M40"/>
-    <mergeCell ref="G41:M41"/>
-    <mergeCell ref="I50:J50"/>
-    <mergeCell ref="I51:J51"/>
-    <mergeCell ref="I52:J52"/>
-    <mergeCell ref="D52:E52"/>
-    <mergeCell ref="G45:M45"/>
-    <mergeCell ref="K50:Q50"/>
-    <mergeCell ref="K51:Q51"/>
-    <mergeCell ref="K52:Q52"/>
+    <mergeCell ref="I53:J53"/>
+    <mergeCell ref="K53:Q53"/>
+    <mergeCell ref="I54:J54"/>
+    <mergeCell ref="K54:Q54"/>
+    <mergeCell ref="I55:J55"/>
+    <mergeCell ref="K55:Q55"/>
+    <mergeCell ref="I59:J59"/>
+    <mergeCell ref="K59:Q59"/>
+    <mergeCell ref="I56:J56"/>
+    <mergeCell ref="K56:Q56"/>
+    <mergeCell ref="I57:J57"/>
+    <mergeCell ref="K57:Q57"/>
+    <mergeCell ref="I58:J58"/>
+    <mergeCell ref="K58:Q58"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
@@ -5577,59 +5576,59 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:22" x14ac:dyDescent="0.2">
-      <c r="A1" s="110" t="s">
+      <c r="A1" s="104" t="s">
         <v>4</v>
       </c>
-      <c r="B1" s="112" t="s">
+      <c r="B1" s="106" t="s">
         <v>5</v>
       </c>
-      <c r="C1" s="113"/>
-      <c r="D1" s="110" t="s">
+      <c r="C1" s="107"/>
+      <c r="D1" s="104" t="s">
         <v>6</v>
       </c>
-      <c r="E1" s="116" t="s">
+      <c r="E1" s="110" t="s">
         <v>7</v>
       </c>
-      <c r="F1" s="116" t="s">
+      <c r="F1" s="110" t="s">
         <v>8</v>
       </c>
-      <c r="G1" s="116" t="s">
+      <c r="G1" s="110" t="s">
         <v>9</v>
       </c>
-      <c r="H1" s="102" t="s">
+      <c r="H1" s="112" t="s">
         <v>10</v>
       </c>
-      <c r="I1" s="103"/>
-      <c r="J1" s="104"/>
-      <c r="K1" s="105" t="s">
+      <c r="I1" s="113"/>
+      <c r="J1" s="114"/>
+      <c r="K1" s="115" t="s">
         <v>11</v>
       </c>
-      <c r="L1" s="103"/>
-      <c r="M1" s="104"/>
-      <c r="N1" s="102" t="s">
-        <v>0</v>
-      </c>
-      <c r="O1" s="103"/>
-      <c r="P1" s="104"/>
-      <c r="Q1" s="105" t="s">
+      <c r="L1" s="113"/>
+      <c r="M1" s="114"/>
+      <c r="N1" s="112" t="s">
+        <v>0</v>
+      </c>
+      <c r="O1" s="113"/>
+      <c r="P1" s="114"/>
+      <c r="Q1" s="115" t="s">
         <v>1</v>
       </c>
-      <c r="R1" s="103"/>
-      <c r="S1" s="104"/>
-      <c r="T1" s="102" t="s">
+      <c r="R1" s="113"/>
+      <c r="S1" s="114"/>
+      <c r="T1" s="112" t="s">
         <v>20</v>
       </c>
-      <c r="U1" s="103"/>
-      <c r="V1" s="104"/>
+      <c r="U1" s="113"/>
+      <c r="V1" s="114"/>
     </row>
     <row r="2" spans="1:22" x14ac:dyDescent="0.2">
-      <c r="A2" s="111"/>
-      <c r="B2" s="114"/>
-      <c r="C2" s="115"/>
-      <c r="D2" s="111"/>
-      <c r="E2" s="117"/>
-      <c r="F2" s="117"/>
-      <c r="G2" s="117"/>
+      <c r="A2" s="105"/>
+      <c r="B2" s="108"/>
+      <c r="C2" s="109"/>
+      <c r="D2" s="105"/>
+      <c r="E2" s="111"/>
+      <c r="F2" s="111"/>
+      <c r="G2" s="111"/>
       <c r="H2" s="2">
         <v>44081</v>
       </c>
@@ -5674,17 +5673,17 @@
       </c>
     </row>
     <row r="3" spans="1:22" x14ac:dyDescent="0.2">
-      <c r="A3" s="111"/>
+      <c r="A3" s="105"/>
       <c r="B3" s="27" t="s">
         <v>2</v>
       </c>
       <c r="C3" s="27" t="s">
         <v>3</v>
       </c>
-      <c r="D3" s="111"/>
-      <c r="E3" s="117"/>
-      <c r="F3" s="117"/>
-      <c r="G3" s="117"/>
+      <c r="D3" s="105"/>
+      <c r="E3" s="111"/>
+      <c r="F3" s="111"/>
+      <c r="G3" s="111"/>
       <c r="H3" s="19" t="s">
         <v>12</v>
       </c>
@@ -7924,15 +7923,15 @@
       <c r="D52" s="39"/>
       <c r="E52" s="26"/>
       <c r="F52" s="37"/>
-      <c r="G52" s="107" t="s">
+      <c r="G52" s="101" t="s">
         <v>114</v>
       </c>
-      <c r="H52" s="108"/>
-      <c r="I52" s="108"/>
-      <c r="J52" s="108"/>
-      <c r="K52" s="108"/>
-      <c r="L52" s="108"/>
-      <c r="M52" s="109"/>
+      <c r="H52" s="102"/>
+      <c r="I52" s="102"/>
+      <c r="J52" s="102"/>
+      <c r="K52" s="102"/>
+      <c r="L52" s="102"/>
+      <c r="M52" s="103"/>
       <c r="N52" s="37"/>
       <c r="O52" s="37"/>
       <c r="P52" s="37"/>
@@ -7959,11 +7958,11 @@
       <c r="M53" s="24"/>
     </row>
     <row r="54" spans="1:22" x14ac:dyDescent="0.2">
-      <c r="A54" s="106"/>
-      <c r="B54" s="106"/>
-      <c r="C54" s="106"/>
-      <c r="D54" s="106"/>
-      <c r="E54" s="106"/>
+      <c r="A54" s="100"/>
+      <c r="B54" s="100"/>
+      <c r="C54" s="100"/>
+      <c r="D54" s="100"/>
+      <c r="E54" s="100"/>
       <c r="F54" s="24"/>
       <c r="G54" s="73"/>
       <c r="H54" s="73"/>
@@ -7974,11 +7973,11 @@
       <c r="M54" s="73"/>
     </row>
     <row r="55" spans="1:22" x14ac:dyDescent="0.2">
-      <c r="A55" s="100"/>
-      <c r="B55" s="101"/>
-      <c r="C55" s="101"/>
-      <c r="D55" s="101"/>
-      <c r="E55" s="101"/>
+      <c r="A55" s="117"/>
+      <c r="B55" s="118"/>
+      <c r="C55" s="118"/>
+      <c r="D55" s="118"/>
+      <c r="E55" s="118"/>
       <c r="F55" s="24"/>
       <c r="G55" s="73"/>
       <c r="H55" s="73"/>
@@ -7989,11 +7988,11 @@
       <c r="M55" s="73"/>
     </row>
     <row r="56" spans="1:22" x14ac:dyDescent="0.2">
-      <c r="A56" s="100"/>
-      <c r="B56" s="101"/>
-      <c r="C56" s="101"/>
-      <c r="D56" s="101"/>
-      <c r="E56" s="101"/>
+      <c r="A56" s="117"/>
+      <c r="B56" s="118"/>
+      <c r="C56" s="118"/>
+      <c r="D56" s="118"/>
+      <c r="E56" s="118"/>
       <c r="F56" s="24"/>
       <c r="G56" s="73"/>
       <c r="H56" s="73"/>
@@ -8004,11 +8003,11 @@
       <c r="M56" s="73"/>
     </row>
     <row r="57" spans="1:22" x14ac:dyDescent="0.2">
-      <c r="A57" s="100"/>
-      <c r="B57" s="101"/>
-      <c r="C57" s="101"/>
-      <c r="D57" s="101"/>
-      <c r="E57" s="101"/>
+      <c r="A57" s="117"/>
+      <c r="B57" s="118"/>
+      <c r="C57" s="118"/>
+      <c r="D57" s="118"/>
+      <c r="E57" s="118"/>
       <c r="F57" s="24"/>
       <c r="G57" s="73"/>
       <c r="H57" s="73"/>
@@ -8025,8 +8024,8 @@
       <c r="D58" s="24"/>
       <c r="E58" s="24"/>
       <c r="F58" s="24"/>
-      <c r="G58" s="101"/>
-      <c r="H58" s="101"/>
+      <c r="G58" s="118"/>
+      <c r="H58" s="118"/>
       <c r="I58" s="73"/>
       <c r="J58" s="73"/>
       <c r="K58" s="73"/>
@@ -8111,10 +8110,10 @@
         <f>E71-E69</f>
         <v>0</v>
       </c>
-      <c r="I65" s="94" t="s">
+      <c r="I65" s="96" t="s">
         <v>28</v>
       </c>
-      <c r="J65" s="94"/>
+      <c r="J65" s="96"/>
       <c r="K65" s="98"/>
       <c r="L65" s="99"/>
       <c r="M65" s="99"/>
@@ -8131,10 +8130,10 @@
         <f>E71-E70</f>
         <v>1.75</v>
       </c>
-      <c r="I66" s="94" t="s">
+      <c r="I66" s="96" t="s">
         <v>29</v>
       </c>
-      <c r="J66" s="94"/>
+      <c r="J66" s="96"/>
       <c r="K66" s="98"/>
       <c r="L66" s="99"/>
       <c r="M66" s="99"/>
@@ -8144,10 +8143,10 @@
       <c r="Q66" s="99"/>
     </row>
     <row r="67" spans="4:19" x14ac:dyDescent="0.2">
-      <c r="D67" s="95" t="s">
+      <c r="D67" s="119" t="s">
         <v>33</v>
       </c>
-      <c r="E67" s="96"/>
+      <c r="E67" s="120"/>
       <c r="G67" s="30" t="s">
         <v>23</v>
       </c>
@@ -8155,10 +8154,10 @@
         <f>E71/E69</f>
         <v>1</v>
       </c>
-      <c r="I67" s="94" t="s">
+      <c r="I67" s="96" t="s">
         <v>31</v>
       </c>
-      <c r="J67" s="94"/>
+      <c r="J67" s="96"/>
       <c r="K67" s="98"/>
       <c r="L67" s="99"/>
       <c r="M67" s="99"/>
@@ -8182,10 +8181,10 @@
         <f>E71/E70</f>
         <v>1.2592592592592593</v>
       </c>
-      <c r="I68" s="94" t="s">
+      <c r="I68" s="96" t="s">
         <v>30</v>
       </c>
-      <c r="J68" s="94"/>
+      <c r="J68" s="96"/>
       <c r="K68" s="98"/>
       <c r="L68" s="99"/>
       <c r="M68" s="99"/>
@@ -8212,10 +8211,10 @@
         <f>E68-E71</f>
         <v>216.5</v>
       </c>
-      <c r="I69" s="94" t="s">
+      <c r="I69" s="96" t="s">
         <v>32</v>
       </c>
-      <c r="J69" s="94"/>
+      <c r="J69" s="96"/>
       <c r="K69" s="98"/>
       <c r="L69" s="99"/>
       <c r="M69" s="99"/>
@@ -8242,10 +8241,10 @@
         <f>(E68-E71)/(H67*H68)</f>
         <v>171.92647058823528</v>
       </c>
-      <c r="I70" s="94" t="s">
+      <c r="I70" s="96" t="s">
         <v>40</v>
       </c>
-      <c r="J70" s="94"/>
+      <c r="J70" s="96"/>
       <c r="K70" s="98"/>
       <c r="L70" s="99"/>
       <c r="M70" s="99"/>
@@ -8272,10 +8271,10 @@
         <f>E70+(E68-E71)</f>
         <v>223.25</v>
       </c>
-      <c r="I71" s="94" t="s">
+      <c r="I71" s="96" t="s">
         <v>34</v>
       </c>
-      <c r="J71" s="94"/>
+      <c r="J71" s="96"/>
       <c r="K71" s="98"/>
       <c r="L71" s="99"/>
       <c r="M71" s="99"/>
@@ -8295,10 +8294,10 @@
         <f>E68/H68</f>
         <v>178.67647058823528</v>
       </c>
-      <c r="I72" s="94" t="s">
+      <c r="I72" s="96" t="s">
         <v>35</v>
       </c>
-      <c r="J72" s="118"/>
+      <c r="J72" s="97"/>
       <c r="K72" s="98"/>
       <c r="L72" s="99"/>
       <c r="M72" s="99"/>
@@ -8319,10 +8318,10 @@
         <f>E70+(E68-E71)/(H67*H68)</f>
         <v>178.67647058823528</v>
       </c>
-      <c r="I73" s="94" t="s">
+      <c r="I73" s="96" t="s">
         <v>41</v>
       </c>
-      <c r="J73" s="118"/>
+      <c r="J73" s="97"/>
       <c r="K73" s="98"/>
       <c r="L73" s="99"/>
       <c r="M73" s="99"/>
@@ -8343,10 +8342,10 @@
         <f>(E68-E71)/(E68-E70)</f>
         <v>0.99198167239404356</v>
       </c>
-      <c r="I74" s="94" t="s">
+      <c r="I74" s="96" t="s">
         <v>42</v>
       </c>
-      <c r="J74" s="118"/>
+      <c r="J74" s="97"/>
       <c r="K74" s="98"/>
       <c r="L74" s="99"/>
       <c r="M74" s="99"/>
@@ -8595,29 +8594,6 @@
     </row>
   </sheetData>
   <mergeCells count="38">
-    <mergeCell ref="I73:J73"/>
-    <mergeCell ref="K73:Q73"/>
-    <mergeCell ref="I74:J74"/>
-    <mergeCell ref="K74:Q74"/>
-    <mergeCell ref="I70:J70"/>
-    <mergeCell ref="K70:Q70"/>
-    <mergeCell ref="I71:J71"/>
-    <mergeCell ref="K71:Q71"/>
-    <mergeCell ref="I72:J72"/>
-    <mergeCell ref="K72:Q72"/>
-    <mergeCell ref="K69:Q69"/>
-    <mergeCell ref="A57:E57"/>
-    <mergeCell ref="G58:H58"/>
-    <mergeCell ref="I65:J65"/>
-    <mergeCell ref="I66:J66"/>
-    <mergeCell ref="K66:Q66"/>
-    <mergeCell ref="D67:E67"/>
-    <mergeCell ref="K65:Q65"/>
-    <mergeCell ref="I67:J67"/>
-    <mergeCell ref="K67:Q67"/>
-    <mergeCell ref="I68:J68"/>
-    <mergeCell ref="K68:Q68"/>
-    <mergeCell ref="I69:J69"/>
     <mergeCell ref="A55:E55"/>
     <mergeCell ref="A56:E56"/>
     <mergeCell ref="T1:V1"/>
@@ -8633,6 +8609,29 @@
     <mergeCell ref="N1:P1"/>
     <mergeCell ref="Q1:S1"/>
     <mergeCell ref="G52:M52"/>
+    <mergeCell ref="K69:Q69"/>
+    <mergeCell ref="A57:E57"/>
+    <mergeCell ref="G58:H58"/>
+    <mergeCell ref="I65:J65"/>
+    <mergeCell ref="I66:J66"/>
+    <mergeCell ref="K66:Q66"/>
+    <mergeCell ref="D67:E67"/>
+    <mergeCell ref="K65:Q65"/>
+    <mergeCell ref="I67:J67"/>
+    <mergeCell ref="K67:Q67"/>
+    <mergeCell ref="I68:J68"/>
+    <mergeCell ref="K68:Q68"/>
+    <mergeCell ref="I69:J69"/>
+    <mergeCell ref="I73:J73"/>
+    <mergeCell ref="K73:Q73"/>
+    <mergeCell ref="I74:J74"/>
+    <mergeCell ref="K74:Q74"/>
+    <mergeCell ref="I70:J70"/>
+    <mergeCell ref="K70:Q70"/>
+    <mergeCell ref="I71:J71"/>
+    <mergeCell ref="K71:Q71"/>
+    <mergeCell ref="I72:J72"/>
+    <mergeCell ref="K72:Q72"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
@@ -8644,8 +8643,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AK152"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="S88" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="AK119" sqref="AK119"/>
+    <sheetView tabSelected="1" topLeftCell="S100" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="M121" sqref="M121"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -8656,84 +8655,84 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:37" x14ac:dyDescent="0.2">
-      <c r="A1" s="110" t="s">
+      <c r="A1" s="104" t="s">
         <v>4</v>
       </c>
-      <c r="B1" s="112" t="s">
+      <c r="B1" s="106" t="s">
         <v>5</v>
       </c>
-      <c r="C1" s="113"/>
-      <c r="D1" s="110" t="s">
+      <c r="C1" s="107"/>
+      <c r="D1" s="104" t="s">
         <v>6</v>
       </c>
-      <c r="E1" s="116" t="s">
+      <c r="E1" s="110" t="s">
         <v>7</v>
       </c>
-      <c r="F1" s="116" t="s">
+      <c r="F1" s="110" t="s">
         <v>8</v>
       </c>
-      <c r="G1" s="116" t="s">
+      <c r="G1" s="110" t="s">
         <v>9</v>
       </c>
-      <c r="H1" s="102" t="s">
+      <c r="H1" s="112" t="s">
         <v>10</v>
       </c>
-      <c r="I1" s="103"/>
-      <c r="J1" s="104"/>
-      <c r="K1" s="105" t="s">
+      <c r="I1" s="113"/>
+      <c r="J1" s="114"/>
+      <c r="K1" s="115" t="s">
         <v>11</v>
       </c>
-      <c r="L1" s="103"/>
-      <c r="M1" s="104"/>
-      <c r="N1" s="102" t="s">
-        <v>0</v>
-      </c>
-      <c r="O1" s="103"/>
-      <c r="P1" s="104"/>
-      <c r="Q1" s="105" t="s">
+      <c r="L1" s="113"/>
+      <c r="M1" s="114"/>
+      <c r="N1" s="112" t="s">
+        <v>0</v>
+      </c>
+      <c r="O1" s="113"/>
+      <c r="P1" s="114"/>
+      <c r="Q1" s="115" t="s">
         <v>1</v>
       </c>
-      <c r="R1" s="103"/>
-      <c r="S1" s="104"/>
-      <c r="T1" s="105" t="s">
+      <c r="R1" s="113"/>
+      <c r="S1" s="114"/>
+      <c r="T1" s="115" t="s">
         <v>231</v>
       </c>
-      <c r="U1" s="103"/>
-      <c r="V1" s="104"/>
-      <c r="W1" s="105" t="s">
+      <c r="U1" s="113"/>
+      <c r="V1" s="114"/>
+      <c r="W1" s="115" t="s">
         <v>232</v>
       </c>
-      <c r="X1" s="103"/>
-      <c r="Y1" s="104"/>
-      <c r="Z1" s="105" t="s">
+      <c r="X1" s="113"/>
+      <c r="Y1" s="114"/>
+      <c r="Z1" s="115" t="s">
         <v>233</v>
       </c>
-      <c r="AA1" s="103"/>
-      <c r="AB1" s="104"/>
-      <c r="AC1" s="105" t="s">
+      <c r="AA1" s="113"/>
+      <c r="AB1" s="114"/>
+      <c r="AC1" s="115" t="s">
         <v>234</v>
       </c>
-      <c r="AD1" s="103"/>
-      <c r="AE1" s="104"/>
-      <c r="AF1" s="105" t="s">
+      <c r="AD1" s="113"/>
+      <c r="AE1" s="114"/>
+      <c r="AF1" s="115" t="s">
         <v>235</v>
       </c>
-      <c r="AG1" s="103"/>
-      <c r="AH1" s="104"/>
-      <c r="AI1" s="102" t="s">
+      <c r="AG1" s="113"/>
+      <c r="AH1" s="114"/>
+      <c r="AI1" s="112" t="s">
         <v>20</v>
       </c>
-      <c r="AJ1" s="103"/>
-      <c r="AK1" s="104"/>
+      <c r="AJ1" s="113"/>
+      <c r="AK1" s="114"/>
     </row>
     <row r="2" spans="1:37" x14ac:dyDescent="0.2">
-      <c r="A2" s="122"/>
-      <c r="B2" s="114"/>
-      <c r="C2" s="115"/>
-      <c r="D2" s="111"/>
-      <c r="E2" s="117"/>
-      <c r="F2" s="117"/>
-      <c r="G2" s="117"/>
+      <c r="A2" s="121"/>
+      <c r="B2" s="108"/>
+      <c r="C2" s="109"/>
+      <c r="D2" s="105"/>
+      <c r="E2" s="111"/>
+      <c r="F2" s="111"/>
+      <c r="G2" s="111"/>
       <c r="H2" s="2">
         <v>44081</v>
       </c>
@@ -8823,17 +8822,17 @@
       </c>
     </row>
     <row r="3" spans="1:37" x14ac:dyDescent="0.2">
-      <c r="A3" s="122"/>
+      <c r="A3" s="121"/>
       <c r="B3" s="76" t="s">
         <v>2</v>
       </c>
       <c r="C3" s="76" t="s">
         <v>3</v>
       </c>
-      <c r="D3" s="111"/>
-      <c r="E3" s="117"/>
-      <c r="F3" s="117"/>
-      <c r="G3" s="117"/>
+      <c r="D3" s="105"/>
+      <c r="E3" s="111"/>
+      <c r="F3" s="111"/>
+      <c r="G3" s="111"/>
       <c r="H3" s="19" t="s">
         <v>12</v>
       </c>
@@ -13077,7 +13076,7 @@
         <v>0</v>
       </c>
       <c r="AK70" s="92">
-        <f t="shared" ref="AK69:AK117" si="5">J70+M70+P70+S70+V70+Y70+AB70+AE70+AH70</f>
+        <f t="shared" ref="AK70:AK117" si="5">J70+M70+P70+S70+V70+Y70+AB70+AE70+AH70</f>
         <v>0</v>
       </c>
     </row>
@@ -14516,7 +14515,7 @@
       <c r="N95" s="82"/>
       <c r="O95" s="82"/>
       <c r="P95" s="82"/>
-      <c r="Q95" s="163"/>
+      <c r="Q95" s="94"/>
       <c r="R95" s="80"/>
       <c r="S95" s="80"/>
       <c r="T95" s="35"/>
@@ -14574,7 +14573,7 @@
       <c r="N96" s="82"/>
       <c r="O96" s="82"/>
       <c r="P96" s="82"/>
-      <c r="Q96" s="163"/>
+      <c r="Q96" s="94"/>
       <c r="R96" s="80"/>
       <c r="S96" s="80"/>
       <c r="T96" s="35"/>
@@ -14630,7 +14629,7 @@
       <c r="N97" s="82"/>
       <c r="O97" s="82"/>
       <c r="P97" s="82"/>
-      <c r="Q97" s="163"/>
+      <c r="Q97" s="94"/>
       <c r="R97" s="80"/>
       <c r="S97" s="80"/>
       <c r="T97" s="35"/>
@@ -15334,7 +15333,7 @@
       <c r="T109" s="35"/>
       <c r="U109" s="35"/>
       <c r="V109" s="35"/>
-      <c r="W109" s="163"/>
+      <c r="W109" s="94"/>
       <c r="X109" s="80"/>
       <c r="Y109" s="80"/>
       <c r="Z109" s="35"/>
@@ -15826,140 +15825,248 @@
     <row r="118" spans="1:37" x14ac:dyDescent="0.2">
       <c r="B118" s="1"/>
       <c r="C118" s="1"/>
-      <c r="E118" s="164" t="s">
+      <c r="E118" s="28" t="s">
         <v>17</v>
       </c>
-      <c r="H118">
-        <f>SUM(H4:H117)</f>
+      <c r="F118" s="28"/>
+      <c r="G118" s="28"/>
+      <c r="H118" s="28">
+        <f t="shared" ref="H118:AK118" si="6">SUM(H4:H117)</f>
         <v>11.5</v>
       </c>
-      <c r="I118">
-        <f>SUM(I4:I117)</f>
+      <c r="I118" s="28">
+        <f t="shared" si="6"/>
         <v>8.5</v>
       </c>
-      <c r="J118">
-        <f>SUM(J4:J117)</f>
+      <c r="J118" s="28">
+        <f t="shared" si="6"/>
         <v>6.75</v>
       </c>
-      <c r="K118">
-        <f>SUM(K4:K117)</f>
+      <c r="K118" s="28">
+        <f t="shared" si="6"/>
         <v>12.5</v>
       </c>
-      <c r="L118">
-        <f>SUM(L4:L117)</f>
+      <c r="L118" s="28">
+        <f t="shared" si="6"/>
         <v>15.5</v>
       </c>
-      <c r="M118">
-        <f>SUM(M4:M117)</f>
+      <c r="M118" s="28">
+        <f t="shared" si="6"/>
         <v>16.75</v>
       </c>
-      <c r="N118">
-        <f>SUM(N4:N117)</f>
+      <c r="N118" s="28">
+        <f t="shared" si="6"/>
         <v>19.5</v>
       </c>
-      <c r="O118">
-        <f>SUM(O4:O117)</f>
+      <c r="O118" s="28">
+        <f t="shared" si="6"/>
         <v>11</v>
       </c>
-      <c r="P118">
-        <f>SUM(P4:P117)</f>
+      <c r="P118" s="28">
+        <f t="shared" si="6"/>
         <v>13</v>
       </c>
-      <c r="Q118">
-        <f>SUM(Q4:Q117)</f>
+      <c r="Q118" s="28">
+        <f t="shared" si="6"/>
         <v>10</v>
       </c>
-      <c r="R118">
-        <f>SUM(R4:R117)</f>
-        <v>0</v>
-      </c>
-      <c r="S118" s="1">
-        <f>SUM(S4:S117)</f>
-        <v>0</v>
-      </c>
-      <c r="T118" s="1">
-        <f>SUM(T4:T117)</f>
-        <v>0</v>
-      </c>
-      <c r="U118" s="1">
-        <f>SUM(U4:U117)</f>
-        <v>0</v>
-      </c>
-      <c r="V118" s="1">
-        <f>SUM(V4:V117)</f>
-        <v>0</v>
-      </c>
-      <c r="W118" s="1">
-        <f>SUM(W4:W117)</f>
+      <c r="R118" s="28">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="S118" s="28">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="T118" s="28">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="U118" s="28">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="V118" s="28">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="W118" s="28">
+        <f t="shared" si="6"/>
         <v>18.5</v>
       </c>
-      <c r="X118" s="1">
-        <f>SUM(X4:X117)</f>
-        <v>0</v>
-      </c>
-      <c r="Y118" s="1">
-        <f>SUM(Y4:Y117)</f>
-        <v>0</v>
-      </c>
-      <c r="Z118" s="1">
-        <f>SUM(Z4:Z117)</f>
+      <c r="X118" s="28">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="Y118" s="28">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="Z118" s="28">
+        <f t="shared" si="6"/>
         <v>2</v>
       </c>
-      <c r="AA118" s="1">
-        <f>SUM(AA4:AA117)</f>
-        <v>0</v>
-      </c>
-      <c r="AB118" s="1">
-        <f>SUM(AB4:AB117)</f>
-        <v>0</v>
-      </c>
-      <c r="AC118" s="1">
-        <f>SUM(AC4:AC117)</f>
+      <c r="AA118" s="28">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="AB118" s="28">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="AC118" s="28">
+        <f t="shared" si="6"/>
         <v>14</v>
       </c>
-      <c r="AD118" s="1">
-        <f>SUM(AD4:AD117)</f>
-        <v>0</v>
-      </c>
-      <c r="AE118" s="1">
-        <f>SUM(AE4:AE117)</f>
-        <v>0</v>
-      </c>
-      <c r="AF118" s="1">
-        <f>SUM(AF4:AF117)</f>
-        <v>0</v>
-      </c>
-      <c r="AG118" s="1">
-        <f>SUM(AG4:AG117)</f>
-        <v>0</v>
-      </c>
-      <c r="AH118" s="1">
-        <f>SUM(AH4:AH117)</f>
-        <v>0</v>
-      </c>
-      <c r="AI118" s="165">
-        <f>SUM(AI4:AI117)</f>
+      <c r="AD118" s="28">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="AE118" s="28">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="AF118" s="28">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="AG118" s="28">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="AH118" s="28">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="AI118" s="95">
+        <f t="shared" si="6"/>
         <v>88</v>
       </c>
-      <c r="AJ118" s="165">
-        <f>SUM(AJ4:AJ117)</f>
+      <c r="AJ118" s="95">
+        <f t="shared" si="6"/>
         <v>35</v>
       </c>
-      <c r="AK118" s="165">
-        <f>SUM(AK4:AK117)</f>
+      <c r="AK118" s="95">
+        <f t="shared" si="6"/>
         <v>36.5</v>
       </c>
     </row>
     <row r="119" spans="1:37" x14ac:dyDescent="0.2">
       <c r="B119" s="1"/>
       <c r="C119" s="1"/>
-      <c r="E119" s="164" t="s">
+      <c r="E119" s="28" t="s">
         <v>18</v>
       </c>
-      <c r="S119" s="1"/>
-      <c r="T119" s="1"/>
-      <c r="U119" s="1"/>
-      <c r="V119" s="1"/>
+      <c r="F119" s="28"/>
+      <c r="G119" s="28"/>
+      <c r="H119" s="28">
+        <f>SUM(H118)</f>
+        <v>11.5</v>
+      </c>
+      <c r="I119" s="28">
+        <f>SUM(I118)</f>
+        <v>8.5</v>
+      </c>
+      <c r="J119" s="28">
+        <f>SUM(J118)</f>
+        <v>6.75</v>
+      </c>
+      <c r="K119" s="28">
+        <f>SUM(K118+H119)</f>
+        <v>24</v>
+      </c>
+      <c r="L119" s="28">
+        <f>SUM(L118+I119)</f>
+        <v>24</v>
+      </c>
+      <c r="M119" s="28">
+        <f>SUM(M118+J119)</f>
+        <v>23.5</v>
+      </c>
+      <c r="N119" s="28">
+        <f>SUM(N118+K119)</f>
+        <v>43.5</v>
+      </c>
+      <c r="O119" s="28">
+        <f>SUM(O118+L119)</f>
+        <v>35</v>
+      </c>
+      <c r="P119" s="28">
+        <f>SUM(P118+M119)</f>
+        <v>36.5</v>
+      </c>
+      <c r="Q119" s="28">
+        <f>SUM(Q118+N119)</f>
+        <v>53.5</v>
+      </c>
+      <c r="R119" s="28">
+        <f>SUM(R118+O119)</f>
+        <v>35</v>
+      </c>
+      <c r="S119" s="28">
+        <f>SUM(S118+P119)</f>
+        <v>36.5</v>
+      </c>
+      <c r="T119" s="28">
+        <f>SUM(T118+Q119)</f>
+        <v>53.5</v>
+      </c>
+      <c r="U119" s="28">
+        <f>SUM(U118+R119)</f>
+        <v>35</v>
+      </c>
+      <c r="V119" s="28">
+        <f>SUM(V118+S119)</f>
+        <v>36.5</v>
+      </c>
+      <c r="W119" s="28">
+        <f>SUM(W118+T119)</f>
+        <v>72</v>
+      </c>
+      <c r="X119" s="28">
+        <f>SUM(X118+U119)</f>
+        <v>35</v>
+      </c>
+      <c r="Y119" s="28">
+        <f>SUM(Y118+V119)</f>
+        <v>36.5</v>
+      </c>
+      <c r="Z119" s="28">
+        <f>SUM(Z118+W119)</f>
+        <v>74</v>
+      </c>
+      <c r="AA119" s="28">
+        <f>SUM(AA118+X119)</f>
+        <v>35</v>
+      </c>
+      <c r="AB119" s="28">
+        <f>SUM(AB118+Y119)</f>
+        <v>36.5</v>
+      </c>
+      <c r="AC119" s="28">
+        <f>SUM(AC118+Z119)</f>
+        <v>88</v>
+      </c>
+      <c r="AD119" s="28">
+        <f>SUM(AD118+AA119)</f>
+        <v>35</v>
+      </c>
+      <c r="AE119" s="28">
+        <f>SUM(AE118+AB119)</f>
+        <v>36.5</v>
+      </c>
+      <c r="AF119" s="28">
+        <f>SUM(AF118+AC119)</f>
+        <v>88</v>
+      </c>
+      <c r="AG119" s="28">
+        <f>SUM(AG118+AD119)</f>
+        <v>35</v>
+      </c>
+      <c r="AH119" s="28">
+        <f>SUM(AH118+AE119)</f>
+        <v>36.5</v>
+      </c>
       <c r="AK119" s="1"/>
     </row>
     <row r="120" spans="1:37" x14ac:dyDescent="0.2">
@@ -16013,19 +16120,19 @@
         <f>E130-E128</f>
         <v>0</v>
       </c>
-      <c r="I124" s="94" t="s">
+      <c r="I124" s="96" t="s">
         <v>28</v>
       </c>
-      <c r="J124" s="94"/>
-      <c r="K124" s="119" t="s">
+      <c r="J124" s="96"/>
+      <c r="K124" s="122" t="s">
         <v>156</v>
       </c>
-      <c r="L124" s="120"/>
-      <c r="M124" s="120"/>
-      <c r="N124" s="120"/>
-      <c r="O124" s="120"/>
-      <c r="P124" s="120"/>
-      <c r="Q124" s="121"/>
+      <c r="L124" s="123"/>
+      <c r="M124" s="123"/>
+      <c r="N124" s="123"/>
+      <c r="O124" s="123"/>
+      <c r="P124" s="123"/>
+      <c r="Q124" s="124"/>
       <c r="S124" s="1"/>
       <c r="T124" s="1"/>
       <c r="U124" s="1"/>
@@ -16045,19 +16152,19 @@
         <f>E130-E129</f>
         <v>0</v>
       </c>
-      <c r="I125" s="94" t="s">
+      <c r="I125" s="96" t="s">
         <v>29</v>
       </c>
-      <c r="J125" s="94"/>
-      <c r="K125" s="119" t="s">
+      <c r="J125" s="96"/>
+      <c r="K125" s="122" t="s">
         <v>157</v>
       </c>
-      <c r="L125" s="120"/>
-      <c r="M125" s="120"/>
-      <c r="N125" s="120"/>
-      <c r="O125" s="120"/>
-      <c r="P125" s="120"/>
-      <c r="Q125" s="121"/>
+      <c r="L125" s="123"/>
+      <c r="M125" s="123"/>
+      <c r="N125" s="123"/>
+      <c r="O125" s="123"/>
+      <c r="P125" s="123"/>
+      <c r="Q125" s="124"/>
       <c r="R125" s="1"/>
       <c r="S125" s="1"/>
       <c r="T125" s="1"/>
@@ -16066,10 +16173,10 @@
       <c r="W125" s="1"/>
     </row>
     <row r="126" spans="1:37" x14ac:dyDescent="0.2">
-      <c r="D126" s="95" t="s">
+      <c r="D126" s="119" t="s">
         <v>158</v>
       </c>
-      <c r="E126" s="96"/>
+      <c r="E126" s="120"/>
       <c r="F126" s="1"/>
       <c r="G126" s="74" t="s">
         <v>23</v>
@@ -16078,19 +16185,19 @@
         <f>E130/E128</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="I126" s="94" t="s">
+      <c r="I126" s="96" t="s">
         <v>31</v>
       </c>
-      <c r="J126" s="94"/>
-      <c r="K126" s="119" t="s">
+      <c r="J126" s="96"/>
+      <c r="K126" s="122" t="s">
         <v>159</v>
       </c>
-      <c r="L126" s="120"/>
-      <c r="M126" s="120"/>
-      <c r="N126" s="120"/>
-      <c r="O126" s="120"/>
-      <c r="P126" s="120"/>
-      <c r="Q126" s="121"/>
+      <c r="L126" s="123"/>
+      <c r="M126" s="123"/>
+      <c r="N126" s="123"/>
+      <c r="O126" s="123"/>
+      <c r="P126" s="123"/>
+      <c r="Q126" s="124"/>
     </row>
     <row r="127" spans="1:37" x14ac:dyDescent="0.2">
       <c r="D127" s="25" t="s">
@@ -16107,19 +16214,19 @@
         <f>E130/E129</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="I127" s="94" t="s">
+      <c r="I127" s="96" t="s">
         <v>30</v>
       </c>
-      <c r="J127" s="94"/>
-      <c r="K127" s="119" t="s">
+      <c r="J127" s="96"/>
+      <c r="K127" s="122" t="s">
         <v>160</v>
       </c>
-      <c r="L127" s="120"/>
-      <c r="M127" s="120"/>
-      <c r="N127" s="120"/>
-      <c r="O127" s="120"/>
-      <c r="P127" s="120"/>
-      <c r="Q127" s="121"/>
+      <c r="L127" s="123"/>
+      <c r="M127" s="123"/>
+      <c r="N127" s="123"/>
+      <c r="O127" s="123"/>
+      <c r="P127" s="123"/>
+      <c r="Q127" s="124"/>
     </row>
     <row r="128" spans="1:37" x14ac:dyDescent="0.2">
       <c r="D128" s="74" t="s">
@@ -16137,19 +16244,19 @@
         <f>E127-E130</f>
         <v>225</v>
       </c>
-      <c r="I128" s="94" t="s">
+      <c r="I128" s="96" t="s">
         <v>32</v>
       </c>
-      <c r="J128" s="94"/>
-      <c r="K128" s="119" t="s">
+      <c r="J128" s="96"/>
+      <c r="K128" s="122" t="s">
         <v>161</v>
       </c>
-      <c r="L128" s="120"/>
-      <c r="M128" s="120"/>
-      <c r="N128" s="120"/>
-      <c r="O128" s="120"/>
-      <c r="P128" s="120"/>
-      <c r="Q128" s="121"/>
+      <c r="L128" s="123"/>
+      <c r="M128" s="123"/>
+      <c r="N128" s="123"/>
+      <c r="O128" s="123"/>
+      <c r="P128" s="123"/>
+      <c r="Q128" s="124"/>
     </row>
     <row r="129" spans="4:17" x14ac:dyDescent="0.2">
       <c r="D129" s="34" t="s">
@@ -16167,19 +16274,19 @@
         <f>(E127-E130)/(H126*H127)</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="I129" s="94" t="s">
+      <c r="I129" s="96" t="s">
         <v>40</v>
       </c>
-      <c r="J129" s="94"/>
-      <c r="K129" s="119" t="s">
+      <c r="J129" s="96"/>
+      <c r="K129" s="122" t="s">
         <v>162</v>
       </c>
-      <c r="L129" s="120"/>
-      <c r="M129" s="120"/>
-      <c r="N129" s="120"/>
-      <c r="O129" s="120"/>
-      <c r="P129" s="120"/>
-      <c r="Q129" s="121"/>
+      <c r="L129" s="123"/>
+      <c r="M129" s="123"/>
+      <c r="N129" s="123"/>
+      <c r="O129" s="123"/>
+      <c r="P129" s="123"/>
+      <c r="Q129" s="124"/>
     </row>
     <row r="130" spans="4:17" x14ac:dyDescent="0.2">
       <c r="D130" s="74" t="s">
@@ -16197,19 +16304,19 @@
         <f>E129+(E127-E130)</f>
         <v>225</v>
       </c>
-      <c r="I130" s="94" t="s">
+      <c r="I130" s="96" t="s">
         <v>34</v>
       </c>
-      <c r="J130" s="94"/>
-      <c r="K130" s="119" t="s">
+      <c r="J130" s="96"/>
+      <c r="K130" s="122" t="s">
         <v>161</v>
       </c>
-      <c r="L130" s="120"/>
-      <c r="M130" s="120"/>
-      <c r="N130" s="120"/>
-      <c r="O130" s="120"/>
-      <c r="P130" s="120"/>
-      <c r="Q130" s="121"/>
+      <c r="L130" s="123"/>
+      <c r="M130" s="123"/>
+      <c r="N130" s="123"/>
+      <c r="O130" s="123"/>
+      <c r="P130" s="123"/>
+      <c r="Q130" s="124"/>
     </row>
     <row r="131" spans="4:17" x14ac:dyDescent="0.2">
       <c r="D131" s="1"/>
@@ -16222,19 +16329,19 @@
         <f>E127/H127</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="I131" s="94" t="s">
+      <c r="I131" s="96" t="s">
         <v>35</v>
       </c>
-      <c r="J131" s="118"/>
-      <c r="K131" s="119" t="s">
+      <c r="J131" s="97"/>
+      <c r="K131" s="122" t="s">
         <v>162</v>
       </c>
-      <c r="L131" s="120"/>
-      <c r="M131" s="120"/>
-      <c r="N131" s="120"/>
-      <c r="O131" s="120"/>
-      <c r="P131" s="120"/>
-      <c r="Q131" s="121"/>
+      <c r="L131" s="123"/>
+      <c r="M131" s="123"/>
+      <c r="N131" s="123"/>
+      <c r="O131" s="123"/>
+      <c r="P131" s="123"/>
+      <c r="Q131" s="124"/>
     </row>
     <row r="132" spans="4:17" x14ac:dyDescent="0.2">
       <c r="D132" s="1"/>
@@ -16247,19 +16354,19 @@
         <f>E129+(E127-E130)/(H126*H127)</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="I132" s="94" t="s">
+      <c r="I132" s="96" t="s">
         <v>41</v>
       </c>
-      <c r="J132" s="118"/>
-      <c r="K132" s="119" t="s">
+      <c r="J132" s="97"/>
+      <c r="K132" s="122" t="s">
         <v>163</v>
       </c>
-      <c r="L132" s="120"/>
-      <c r="M132" s="120"/>
-      <c r="N132" s="120"/>
-      <c r="O132" s="120"/>
-      <c r="P132" s="120"/>
-      <c r="Q132" s="121"/>
+      <c r="L132" s="123"/>
+      <c r="M132" s="123"/>
+      <c r="N132" s="123"/>
+      <c r="O132" s="123"/>
+      <c r="P132" s="123"/>
+      <c r="Q132" s="124"/>
     </row>
     <row r="133" spans="4:17" x14ac:dyDescent="0.2">
       <c r="D133" s="1"/>
@@ -16272,19 +16379,19 @@
         <f>(E127-E130)/(E127-E129)</f>
         <v>1</v>
       </c>
-      <c r="I133" s="94" t="s">
+      <c r="I133" s="96" t="s">
         <v>42</v>
       </c>
-      <c r="J133" s="118"/>
-      <c r="K133" s="119" t="s">
+      <c r="J133" s="97"/>
+      <c r="K133" s="122" t="s">
         <v>164</v>
       </c>
-      <c r="L133" s="120"/>
-      <c r="M133" s="120"/>
-      <c r="N133" s="120"/>
-      <c r="O133" s="120"/>
-      <c r="P133" s="120"/>
-      <c r="Q133" s="121"/>
+      <c r="L133" s="123"/>
+      <c r="M133" s="123"/>
+      <c r="N133" s="123"/>
+      <c r="O133" s="123"/>
+      <c r="P133" s="123"/>
+      <c r="Q133" s="124"/>
     </row>
     <row r="134" spans="4:17" x14ac:dyDescent="0.2">
       <c r="D134" s="1"/>
@@ -16633,13 +16740,25 @@
     </row>
   </sheetData>
   <mergeCells count="37">
-    <mergeCell ref="G1:G3"/>
-    <mergeCell ref="H1:J1"/>
-    <mergeCell ref="A1:A3"/>
-    <mergeCell ref="B1:C2"/>
-    <mergeCell ref="D1:D3"/>
-    <mergeCell ref="E1:E3"/>
-    <mergeCell ref="F1:F3"/>
+    <mergeCell ref="I133:J133"/>
+    <mergeCell ref="K133:Q133"/>
+    <mergeCell ref="I130:J130"/>
+    <mergeCell ref="K130:Q130"/>
+    <mergeCell ref="I131:J131"/>
+    <mergeCell ref="K131:Q131"/>
+    <mergeCell ref="I132:J132"/>
+    <mergeCell ref="K132:Q132"/>
+    <mergeCell ref="I127:J127"/>
+    <mergeCell ref="K127:Q127"/>
+    <mergeCell ref="I128:J128"/>
+    <mergeCell ref="K128:Q128"/>
+    <mergeCell ref="I129:J129"/>
+    <mergeCell ref="K129:Q129"/>
+    <mergeCell ref="I125:J125"/>
+    <mergeCell ref="K125:Q125"/>
+    <mergeCell ref="D126:E126"/>
+    <mergeCell ref="I126:J126"/>
+    <mergeCell ref="K126:Q126"/>
     <mergeCell ref="K1:M1"/>
     <mergeCell ref="N1:P1"/>
     <mergeCell ref="Q1:S1"/>
@@ -16651,25 +16770,13 @@
     <mergeCell ref="AC1:AE1"/>
     <mergeCell ref="AF1:AH1"/>
     <mergeCell ref="K124:Q124"/>
-    <mergeCell ref="I125:J125"/>
-    <mergeCell ref="K125:Q125"/>
-    <mergeCell ref="D126:E126"/>
-    <mergeCell ref="I126:J126"/>
-    <mergeCell ref="K126:Q126"/>
-    <mergeCell ref="I127:J127"/>
-    <mergeCell ref="K127:Q127"/>
-    <mergeCell ref="I128:J128"/>
-    <mergeCell ref="K128:Q128"/>
-    <mergeCell ref="I129:J129"/>
-    <mergeCell ref="K129:Q129"/>
-    <mergeCell ref="I133:J133"/>
-    <mergeCell ref="K133:Q133"/>
-    <mergeCell ref="I130:J130"/>
-    <mergeCell ref="K130:Q130"/>
-    <mergeCell ref="I131:J131"/>
-    <mergeCell ref="K131:Q131"/>
-    <mergeCell ref="I132:J132"/>
-    <mergeCell ref="K132:Q132"/>
+    <mergeCell ref="G1:G3"/>
+    <mergeCell ref="H1:J1"/>
+    <mergeCell ref="A1:A3"/>
+    <mergeCell ref="B1:C2"/>
+    <mergeCell ref="D1:D3"/>
+    <mergeCell ref="E1:E3"/>
+    <mergeCell ref="F1:F3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
@@ -16694,105 +16801,105 @@
   <sheetData>
     <row r="1" spans="1:10" ht="13.5" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="2" spans="1:10" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="143" t="s">
+      <c r="A2" s="125" t="s">
         <v>116</v>
       </c>
-      <c r="B2" s="143"/>
-      <c r="C2" s="143"/>
-      <c r="D2" s="143"/>
-      <c r="E2" s="143"/>
-      <c r="F2" s="143"/>
-      <c r="G2" s="143"/>
-      <c r="H2" s="143"/>
-      <c r="I2" s="143"/>
-      <c r="J2" s="143"/>
+      <c r="B2" s="125"/>
+      <c r="C2" s="125"/>
+      <c r="D2" s="125"/>
+      <c r="E2" s="125"/>
+      <c r="F2" s="125"/>
+      <c r="G2" s="125"/>
+      <c r="H2" s="125"/>
+      <c r="I2" s="125"/>
+      <c r="J2" s="125"/>
     </row>
     <row r="3" spans="1:10" ht="26.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A3" s="72" t="s">
         <v>43</v>
       </c>
-      <c r="B3" s="151" t="s">
+      <c r="B3" s="135" t="s">
         <v>108</v>
       </c>
-      <c r="C3" s="152"/>
-      <c r="D3" s="152"/>
-      <c r="E3" s="152"/>
-      <c r="F3" s="152"/>
-      <c r="G3" s="152"/>
-      <c r="H3" s="152"/>
-      <c r="I3" s="152"/>
-      <c r="J3" s="153"/>
+      <c r="C3" s="136"/>
+      <c r="D3" s="136"/>
+      <c r="E3" s="136"/>
+      <c r="F3" s="136"/>
+      <c r="G3" s="136"/>
+      <c r="H3" s="136"/>
+      <c r="I3" s="136"/>
+      <c r="J3" s="137"/>
     </row>
     <row r="4" spans="1:10" ht="18.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A4" s="72" t="s">
         <v>44</v>
       </c>
-      <c r="B4" s="151" t="s">
+      <c r="B4" s="135" t="s">
         <v>107</v>
       </c>
-      <c r="C4" s="152"/>
-      <c r="D4" s="152"/>
-      <c r="E4" s="152"/>
-      <c r="F4" s="152"/>
-      <c r="G4" s="152"/>
-      <c r="H4" s="152"/>
-      <c r="I4" s="152"/>
-      <c r="J4" s="153"/>
+      <c r="C4" s="136"/>
+      <c r="D4" s="136"/>
+      <c r="E4" s="136"/>
+      <c r="F4" s="136"/>
+      <c r="G4" s="136"/>
+      <c r="H4" s="136"/>
+      <c r="I4" s="136"/>
+      <c r="J4" s="137"/>
     </row>
     <row r="5" spans="1:10" ht="26.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A5" s="72" t="s">
         <v>45</v>
       </c>
-      <c r="B5" s="151" t="s">
+      <c r="B5" s="135" t="s">
         <v>115</v>
       </c>
-      <c r="C5" s="152"/>
-      <c r="D5" s="152"/>
-      <c r="E5" s="152"/>
-      <c r="F5" s="152"/>
-      <c r="G5" s="152"/>
-      <c r="H5" s="152"/>
-      <c r="I5" s="152"/>
-      <c r="J5" s="153"/>
+      <c r="C5" s="136"/>
+      <c r="D5" s="136"/>
+      <c r="E5" s="136"/>
+      <c r="F5" s="136"/>
+      <c r="G5" s="136"/>
+      <c r="H5" s="136"/>
+      <c r="I5" s="136"/>
+      <c r="J5" s="137"/>
     </row>
     <row r="25" spans="2:11" ht="13.5" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="26" spans="2:11" ht="17.45" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B26" s="126" t="s">
+      <c r="B26" s="138" t="s">
         <v>168</v>
       </c>
-      <c r="C26" s="127"/>
-      <c r="D26" s="127"/>
-      <c r="E26" s="127"/>
-      <c r="F26" s="127"/>
-      <c r="G26" s="127"/>
-      <c r="H26" s="127"/>
-      <c r="I26" s="127"/>
-      <c r="J26" s="127"/>
-      <c r="K26" s="128"/>
+      <c r="C26" s="139"/>
+      <c r="D26" s="139"/>
+      <c r="E26" s="139"/>
+      <c r="F26" s="139"/>
+      <c r="G26" s="139"/>
+      <c r="H26" s="139"/>
+      <c r="I26" s="139"/>
+      <c r="J26" s="139"/>
+      <c r="K26" s="140"/>
     </row>
     <row r="27" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B27" s="129"/>
-      <c r="C27" s="130"/>
-      <c r="D27" s="130"/>
-      <c r="E27" s="130"/>
-      <c r="F27" s="130"/>
-      <c r="G27" s="130"/>
-      <c r="H27" s="130"/>
-      <c r="I27" s="130"/>
-      <c r="J27" s="130"/>
-      <c r="K27" s="131"/>
+      <c r="B27" s="141"/>
+      <c r="C27" s="142"/>
+      <c r="D27" s="142"/>
+      <c r="E27" s="142"/>
+      <c r="F27" s="142"/>
+      <c r="G27" s="142"/>
+      <c r="H27" s="142"/>
+      <c r="I27" s="142"/>
+      <c r="J27" s="142"/>
+      <c r="K27" s="143"/>
     </row>
     <row r="28" spans="2:11" ht="13.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B28" s="132"/>
-      <c r="C28" s="133"/>
-      <c r="D28" s="133"/>
-      <c r="E28" s="133"/>
-      <c r="F28" s="133"/>
-      <c r="G28" s="133"/>
-      <c r="H28" s="133"/>
-      <c r="I28" s="133"/>
-      <c r="J28" s="133"/>
-      <c r="K28" s="134"/>
+      <c r="B28" s="144"/>
+      <c r="C28" s="145"/>
+      <c r="D28" s="145"/>
+      <c r="E28" s="145"/>
+      <c r="F28" s="145"/>
+      <c r="G28" s="145"/>
+      <c r="H28" s="145"/>
+      <c r="I28" s="145"/>
+      <c r="J28" s="145"/>
+      <c r="K28" s="146"/>
     </row>
     <row r="29" spans="2:11" ht="13.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B29" s="60"/>
@@ -16806,18 +16913,18 @@
       <c r="J29" s="60"/>
     </row>
     <row r="30" spans="2:11" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B30" s="154" t="s">
+      <c r="B30" s="147" t="s">
         <v>116</v>
       </c>
-      <c r="C30" s="155"/>
-      <c r="D30" s="155"/>
-      <c r="E30" s="155"/>
-      <c r="F30" s="155"/>
-      <c r="G30" s="155"/>
-      <c r="H30" s="155"/>
-      <c r="I30" s="155"/>
-      <c r="J30" s="155"/>
-      <c r="K30" s="156"/>
+      <c r="C30" s="148"/>
+      <c r="D30" s="148"/>
+      <c r="E30" s="148"/>
+      <c r="F30" s="148"/>
+      <c r="G30" s="148"/>
+      <c r="H30" s="148"/>
+      <c r="I30" s="148"/>
+      <c r="J30" s="148"/>
+      <c r="K30" s="149"/>
     </row>
     <row r="31" spans="2:11" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B31" s="61"/>
@@ -16854,22 +16961,22 @@
       <c r="K33" s="61"/>
     </row>
     <row r="34" spans="2:11" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B34" s="144" t="s">
+      <c r="B34" s="128" t="s">
         <v>46</v>
       </c>
-      <c r="C34" s="145"/>
-      <c r="D34" s="144" t="s">
+      <c r="C34" s="129"/>
+      <c r="D34" s="128" t="s">
         <v>47</v>
       </c>
-      <c r="E34" s="145"/>
-      <c r="F34" s="144" t="s">
+      <c r="E34" s="129"/>
+      <c r="F34" s="128" t="s">
         <v>106</v>
       </c>
-      <c r="G34" s="150"/>
-      <c r="H34" s="150"/>
-      <c r="I34" s="150"/>
-      <c r="J34" s="150"/>
-      <c r="K34" s="145"/>
+      <c r="G34" s="134"/>
+      <c r="H34" s="134"/>
+      <c r="I34" s="134"/>
+      <c r="J34" s="134"/>
+      <c r="K34" s="129"/>
     </row>
     <row r="35" spans="2:11" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B35" s="62" t="s">
@@ -16878,16 +16985,16 @@
       <c r="C35" s="71">
         <v>225</v>
       </c>
-      <c r="D35" s="146" t="s">
+      <c r="D35" s="130" t="s">
         <v>165</v>
       </c>
-      <c r="E35" s="147"/>
-      <c r="F35" s="135"/>
-      <c r="G35" s="136"/>
-      <c r="H35" s="136"/>
-      <c r="I35" s="136"/>
-      <c r="J35" s="136"/>
-      <c r="K35" s="137"/>
+      <c r="E35" s="131"/>
+      <c r="F35" s="150"/>
+      <c r="G35" s="155"/>
+      <c r="H35" s="155"/>
+      <c r="I35" s="155"/>
+      <c r="J35" s="155"/>
+      <c r="K35" s="151"/>
     </row>
     <row r="36" spans="2:11" ht="13.9" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B36" s="62" t="s">
@@ -16896,14 +17003,14 @@
       <c r="C36" s="70">
         <v>8.5</v>
       </c>
-      <c r="D36" s="148"/>
-      <c r="E36" s="149"/>
-      <c r="F36" s="135"/>
-      <c r="G36" s="136"/>
-      <c r="H36" s="136"/>
-      <c r="I36" s="136"/>
-      <c r="J36" s="136"/>
-      <c r="K36" s="137"/>
+      <c r="D36" s="132"/>
+      <c r="E36" s="133"/>
+      <c r="F36" s="150"/>
+      <c r="G36" s="155"/>
+      <c r="H36" s="155"/>
+      <c r="I36" s="155"/>
+      <c r="J36" s="155"/>
+      <c r="K36" s="151"/>
     </row>
     <row r="37" spans="2:11" ht="57" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B37" s="62" t="s">
@@ -16912,16 +17019,16 @@
       <c r="C37" s="63">
         <v>6.75</v>
       </c>
-      <c r="D37" s="135"/>
-      <c r="E37" s="137"/>
-      <c r="F37" s="140" t="s">
+      <c r="D37" s="150"/>
+      <c r="E37" s="151"/>
+      <c r="F37" s="152" t="s">
         <v>111</v>
       </c>
-      <c r="G37" s="141"/>
-      <c r="H37" s="141"/>
-      <c r="I37" s="141"/>
-      <c r="J37" s="141"/>
-      <c r="K37" s="142"/>
+      <c r="G37" s="153"/>
+      <c r="H37" s="153"/>
+      <c r="I37" s="153"/>
+      <c r="J37" s="153"/>
+      <c r="K37" s="154"/>
     </row>
     <row r="38" spans="2:11" ht="32.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B38" s="62" t="s">
@@ -16930,16 +17037,16 @@
       <c r="C38" s="63">
         <v>8.5</v>
       </c>
-      <c r="D38" s="135"/>
-      <c r="E38" s="137"/>
-      <c r="F38" s="140" t="s">
+      <c r="D38" s="150"/>
+      <c r="E38" s="151"/>
+      <c r="F38" s="152" t="s">
         <v>112</v>
       </c>
-      <c r="G38" s="141"/>
-      <c r="H38" s="141"/>
-      <c r="I38" s="141"/>
-      <c r="J38" s="141"/>
-      <c r="K38" s="142"/>
+      <c r="G38" s="153"/>
+      <c r="H38" s="153"/>
+      <c r="I38" s="153"/>
+      <c r="J38" s="153"/>
+      <c r="K38" s="154"/>
     </row>
     <row r="39" spans="2:11" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B39" s="62" t="s">
@@ -16948,18 +17055,18 @@
       <c r="C39" s="63">
         <v>0</v>
       </c>
-      <c r="D39" s="138" t="s">
+      <c r="D39" s="126" t="s">
         <v>28</v>
       </c>
-      <c r="E39" s="139"/>
-      <c r="F39" s="140" t="s">
+      <c r="E39" s="127"/>
+      <c r="F39" s="152" t="s">
         <v>109</v>
       </c>
-      <c r="G39" s="141"/>
-      <c r="H39" s="141"/>
-      <c r="I39" s="141"/>
-      <c r="J39" s="141"/>
-      <c r="K39" s="142"/>
+      <c r="G39" s="153"/>
+      <c r="H39" s="153"/>
+      <c r="I39" s="153"/>
+      <c r="J39" s="153"/>
+      <c r="K39" s="154"/>
     </row>
     <row r="40" spans="2:11" ht="36.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B40" s="62" t="s">
@@ -16968,18 +17075,18 @@
       <c r="C40" s="63">
         <v>1.75</v>
       </c>
-      <c r="D40" s="138" t="s">
+      <c r="D40" s="126" t="s">
         <v>29</v>
       </c>
-      <c r="E40" s="139"/>
-      <c r="F40" s="140" t="s">
+      <c r="E40" s="127"/>
+      <c r="F40" s="152" t="s">
         <v>117</v>
       </c>
-      <c r="G40" s="141"/>
-      <c r="H40" s="141"/>
-      <c r="I40" s="141"/>
-      <c r="J40" s="141"/>
-      <c r="K40" s="142"/>
+      <c r="G40" s="153"/>
+      <c r="H40" s="153"/>
+      <c r="I40" s="153"/>
+      <c r="J40" s="153"/>
+      <c r="K40" s="154"/>
     </row>
     <row r="41" spans="2:11" ht="27" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B41" s="62" t="s">
@@ -16988,18 +17095,18 @@
       <c r="C41" s="63">
         <v>1</v>
       </c>
-      <c r="D41" s="138" t="s">
+      <c r="D41" s="126" t="s">
         <v>31</v>
       </c>
-      <c r="E41" s="139"/>
-      <c r="F41" s="140" t="s">
+      <c r="E41" s="127"/>
+      <c r="F41" s="152" t="s">
         <v>110</v>
       </c>
-      <c r="G41" s="141"/>
-      <c r="H41" s="141"/>
-      <c r="I41" s="141"/>
-      <c r="J41" s="141"/>
-      <c r="K41" s="142"/>
+      <c r="G41" s="153"/>
+      <c r="H41" s="153"/>
+      <c r="I41" s="153"/>
+      <c r="J41" s="153"/>
+      <c r="K41" s="154"/>
     </row>
     <row r="42" spans="2:11" ht="55.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B42" s="62" t="s">
@@ -17008,18 +17115,18 @@
       <c r="C42" s="63">
         <v>1.26</v>
       </c>
-      <c r="D42" s="138" t="s">
+      <c r="D42" s="126" t="s">
         <v>30</v>
       </c>
-      <c r="E42" s="139"/>
-      <c r="F42" s="140" t="s">
+      <c r="E42" s="127"/>
+      <c r="F42" s="152" t="s">
         <v>118</v>
       </c>
-      <c r="G42" s="141"/>
-      <c r="H42" s="141"/>
-      <c r="I42" s="141"/>
-      <c r="J42" s="141"/>
-      <c r="K42" s="142"/>
+      <c r="G42" s="153"/>
+      <c r="H42" s="153"/>
+      <c r="I42" s="153"/>
+      <c r="J42" s="153"/>
+      <c r="K42" s="154"/>
     </row>
     <row r="43" spans="2:11" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B43" s="62" t="s">
@@ -17028,18 +17135,18 @@
       <c r="C43" s="63">
         <v>15.5</v>
       </c>
-      <c r="D43" s="138" t="s">
+      <c r="D43" s="126" t="s">
         <v>32</v>
       </c>
-      <c r="E43" s="139"/>
-      <c r="F43" s="140" t="s">
+      <c r="E43" s="127"/>
+      <c r="F43" s="152" t="s">
         <v>119</v>
       </c>
-      <c r="G43" s="141"/>
-      <c r="H43" s="141"/>
-      <c r="I43" s="141"/>
-      <c r="J43" s="141"/>
-      <c r="K43" s="142"/>
+      <c r="G43" s="153"/>
+      <c r="H43" s="153"/>
+      <c r="I43" s="153"/>
+      <c r="J43" s="153"/>
+      <c r="K43" s="154"/>
     </row>
     <row r="44" spans="2:11" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B44" s="62" t="s">
@@ -17048,18 +17155,18 @@
       <c r="C44" s="63">
         <v>12.31</v>
       </c>
-      <c r="D44" s="138" t="s">
+      <c r="D44" s="126" t="s">
         <v>40</v>
       </c>
-      <c r="E44" s="139"/>
-      <c r="F44" s="140" t="s">
+      <c r="E44" s="127"/>
+      <c r="F44" s="152" t="s">
         <v>120</v>
       </c>
-      <c r="G44" s="141"/>
-      <c r="H44" s="141"/>
-      <c r="I44" s="141"/>
-      <c r="J44" s="141"/>
-      <c r="K44" s="142"/>
+      <c r="G44" s="153"/>
+      <c r="H44" s="153"/>
+      <c r="I44" s="153"/>
+      <c r="J44" s="153"/>
+      <c r="K44" s="154"/>
     </row>
     <row r="45" spans="2:11" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B45" s="62" t="s">
@@ -17068,18 +17175,18 @@
       <c r="C45" s="63">
         <v>22.25</v>
       </c>
-      <c r="D45" s="138" t="s">
+      <c r="D45" s="126" t="s">
         <v>34</v>
       </c>
-      <c r="E45" s="139"/>
-      <c r="F45" s="135" t="s">
+      <c r="E45" s="127"/>
+      <c r="F45" s="150" t="s">
         <v>121</v>
       </c>
-      <c r="G45" s="136"/>
-      <c r="H45" s="136"/>
-      <c r="I45" s="136"/>
-      <c r="J45" s="136"/>
-      <c r="K45" s="137"/>
+      <c r="G45" s="155"/>
+      <c r="H45" s="155"/>
+      <c r="I45" s="155"/>
+      <c r="J45" s="155"/>
+      <c r="K45" s="151"/>
     </row>
     <row r="46" spans="2:11" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B46" s="62" t="s">
@@ -17088,18 +17195,18 @@
       <c r="C46" s="63">
         <v>19.059999999999999</v>
       </c>
-      <c r="D46" s="138" t="s">
+      <c r="D46" s="126" t="s">
         <v>35</v>
       </c>
-      <c r="E46" s="139"/>
-      <c r="F46" s="135" t="s">
+      <c r="E46" s="127"/>
+      <c r="F46" s="150" t="s">
         <v>121</v>
       </c>
-      <c r="G46" s="136"/>
-      <c r="H46" s="136"/>
-      <c r="I46" s="136"/>
-      <c r="J46" s="136"/>
-      <c r="K46" s="137"/>
+      <c r="G46" s="155"/>
+      <c r="H46" s="155"/>
+      <c r="I46" s="155"/>
+      <c r="J46" s="155"/>
+      <c r="K46" s="151"/>
     </row>
     <row r="47" spans="2:11" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B47" s="62" t="s">
@@ -17108,18 +17215,18 @@
       <c r="C47" s="63">
         <v>19.059999999999999</v>
       </c>
-      <c r="D47" s="138" t="s">
+      <c r="D47" s="126" t="s">
         <v>41</v>
       </c>
-      <c r="E47" s="139"/>
-      <c r="F47" s="135" t="s">
+      <c r="E47" s="127"/>
+      <c r="F47" s="150" t="s">
         <v>121</v>
       </c>
-      <c r="G47" s="136"/>
-      <c r="H47" s="136"/>
-      <c r="I47" s="136"/>
-      <c r="J47" s="136"/>
-      <c r="K47" s="137"/>
+      <c r="G47" s="155"/>
+      <c r="H47" s="155"/>
+      <c r="I47" s="155"/>
+      <c r="J47" s="155"/>
+      <c r="K47" s="151"/>
     </row>
     <row r="48" spans="2:11" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B48" s="62" t="s">
@@ -17128,66 +17235,66 @@
       <c r="C48" s="63">
         <v>0.9</v>
       </c>
-      <c r="D48" s="138" t="s">
+      <c r="D48" s="126" t="s">
         <v>42</v>
       </c>
-      <c r="E48" s="139"/>
-      <c r="F48" s="135"/>
-      <c r="G48" s="136"/>
-      <c r="H48" s="136"/>
-      <c r="I48" s="136"/>
-      <c r="J48" s="136"/>
-      <c r="K48" s="137"/>
+      <c r="E48" s="127"/>
+      <c r="F48" s="150"/>
+      <c r="G48" s="155"/>
+      <c r="H48" s="155"/>
+      <c r="I48" s="155"/>
+      <c r="J48" s="155"/>
+      <c r="K48" s="151"/>
     </row>
     <row r="49" spans="2:11" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B49" s="60"/>
       <c r="C49" s="60"/>
       <c r="D49" s="60"/>
       <c r="E49" s="60"/>
-      <c r="F49" s="123"/>
-      <c r="G49" s="124"/>
-      <c r="H49" s="124"/>
-      <c r="I49" s="124"/>
-      <c r="J49" s="124"/>
-      <c r="K49" s="125"/>
+      <c r="F49" s="156"/>
+      <c r="G49" s="157"/>
+      <c r="H49" s="157"/>
+      <c r="I49" s="157"/>
+      <c r="J49" s="157"/>
+      <c r="K49" s="158"/>
     </row>
     <row r="50" spans="2:11" ht="17.45" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B50" s="126" t="s">
+      <c r="B50" s="138" t="s">
         <v>113</v>
       </c>
-      <c r="C50" s="127"/>
-      <c r="D50" s="127"/>
-      <c r="E50" s="127"/>
-      <c r="F50" s="127"/>
-      <c r="G50" s="127"/>
-      <c r="H50" s="127"/>
-      <c r="I50" s="127"/>
-      <c r="J50" s="127"/>
-      <c r="K50" s="128"/>
+      <c r="C50" s="139"/>
+      <c r="D50" s="139"/>
+      <c r="E50" s="139"/>
+      <c r="F50" s="139"/>
+      <c r="G50" s="139"/>
+      <c r="H50" s="139"/>
+      <c r="I50" s="139"/>
+      <c r="J50" s="139"/>
+      <c r="K50" s="140"/>
     </row>
     <row r="51" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B51" s="129"/>
-      <c r="C51" s="130"/>
-      <c r="D51" s="130"/>
-      <c r="E51" s="130"/>
-      <c r="F51" s="130"/>
-      <c r="G51" s="130"/>
-      <c r="H51" s="130"/>
-      <c r="I51" s="130"/>
-      <c r="J51" s="130"/>
-      <c r="K51" s="131"/>
+      <c r="B51" s="141"/>
+      <c r="C51" s="142"/>
+      <c r="D51" s="142"/>
+      <c r="E51" s="142"/>
+      <c r="F51" s="142"/>
+      <c r="G51" s="142"/>
+      <c r="H51" s="142"/>
+      <c r="I51" s="142"/>
+      <c r="J51" s="142"/>
+      <c r="K51" s="143"/>
     </row>
     <row r="52" spans="2:11" ht="13.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B52" s="132"/>
-      <c r="C52" s="133"/>
-      <c r="D52" s="133"/>
-      <c r="E52" s="133"/>
-      <c r="F52" s="133"/>
-      <c r="G52" s="133"/>
-      <c r="H52" s="133"/>
-      <c r="I52" s="133"/>
-      <c r="J52" s="133"/>
-      <c r="K52" s="134"/>
+      <c r="B52" s="144"/>
+      <c r="C52" s="145"/>
+      <c r="D52" s="145"/>
+      <c r="E52" s="145"/>
+      <c r="F52" s="145"/>
+      <c r="G52" s="145"/>
+      <c r="H52" s="145"/>
+      <c r="I52" s="145"/>
+      <c r="J52" s="145"/>
+      <c r="K52" s="146"/>
     </row>
     <row r="53" spans="2:11" ht="13.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B53" s="61"/>
@@ -17242,6 +17349,31 @@
     </row>
   </sheetData>
   <mergeCells count="39">
+    <mergeCell ref="F49:K49"/>
+    <mergeCell ref="B50:K52"/>
+    <mergeCell ref="F47:K47"/>
+    <mergeCell ref="D47:E47"/>
+    <mergeCell ref="D48:E48"/>
+    <mergeCell ref="F48:K48"/>
+    <mergeCell ref="D43:E43"/>
+    <mergeCell ref="F43:K43"/>
+    <mergeCell ref="F35:K35"/>
+    <mergeCell ref="F36:K36"/>
+    <mergeCell ref="F38:K38"/>
+    <mergeCell ref="F39:K39"/>
+    <mergeCell ref="D40:E40"/>
+    <mergeCell ref="D41:E41"/>
+    <mergeCell ref="D42:E42"/>
+    <mergeCell ref="F40:K40"/>
+    <mergeCell ref="F41:K41"/>
+    <mergeCell ref="F42:K42"/>
+    <mergeCell ref="F37:K37"/>
+    <mergeCell ref="F44:K44"/>
+    <mergeCell ref="F45:K45"/>
+    <mergeCell ref="F46:K46"/>
+    <mergeCell ref="D46:E46"/>
+    <mergeCell ref="D44:E44"/>
+    <mergeCell ref="D45:E45"/>
     <mergeCell ref="A2:J2"/>
     <mergeCell ref="D39:E39"/>
     <mergeCell ref="B34:C34"/>
@@ -17256,31 +17388,6 @@
     <mergeCell ref="B30:K30"/>
     <mergeCell ref="D37:E37"/>
     <mergeCell ref="D38:E38"/>
-    <mergeCell ref="F44:K44"/>
-    <mergeCell ref="F45:K45"/>
-    <mergeCell ref="F46:K46"/>
-    <mergeCell ref="D46:E46"/>
-    <mergeCell ref="D44:E44"/>
-    <mergeCell ref="D45:E45"/>
-    <mergeCell ref="D43:E43"/>
-    <mergeCell ref="F43:K43"/>
-    <mergeCell ref="F35:K35"/>
-    <mergeCell ref="F36:K36"/>
-    <mergeCell ref="F38:K38"/>
-    <mergeCell ref="F39:K39"/>
-    <mergeCell ref="D40:E40"/>
-    <mergeCell ref="D41:E41"/>
-    <mergeCell ref="D42:E42"/>
-    <mergeCell ref="F40:K40"/>
-    <mergeCell ref="F41:K41"/>
-    <mergeCell ref="F42:K42"/>
-    <mergeCell ref="F37:K37"/>
-    <mergeCell ref="F49:K49"/>
-    <mergeCell ref="B50:K52"/>
-    <mergeCell ref="F47:K47"/>
-    <mergeCell ref="D47:E47"/>
-    <mergeCell ref="D48:E48"/>
-    <mergeCell ref="F48:K48"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
@@ -17309,98 +17416,98 @@
   <sheetData>
     <row r="1" spans="1:9" ht="13.5" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="2" spans="1:9" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="143" t="s">
+      <c r="A2" s="125" t="s">
         <v>166</v>
       </c>
-      <c r="B2" s="143"/>
-      <c r="C2" s="143"/>
-      <c r="D2" s="143"/>
-      <c r="E2" s="143"/>
-      <c r="F2" s="143"/>
-      <c r="G2" s="143"/>
-      <c r="H2" s="143"/>
-      <c r="I2" s="143"/>
+      <c r="B2" s="125"/>
+      <c r="C2" s="125"/>
+      <c r="D2" s="125"/>
+      <c r="E2" s="125"/>
+      <c r="F2" s="125"/>
+      <c r="G2" s="125"/>
+      <c r="H2" s="125"/>
+      <c r="I2" s="125"/>
     </row>
     <row r="3" spans="1:9" ht="26.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A3" s="72" t="s">
         <v>43</v>
       </c>
-      <c r="B3" s="151" t="s">
+      <c r="B3" s="135" t="s">
         <v>108</v>
       </c>
-      <c r="C3" s="152"/>
-      <c r="D3" s="152"/>
-      <c r="E3" s="152"/>
-      <c r="F3" s="152"/>
-      <c r="G3" s="152"/>
-      <c r="H3" s="152"/>
-      <c r="I3" s="153"/>
+      <c r="C3" s="136"/>
+      <c r="D3" s="136"/>
+      <c r="E3" s="136"/>
+      <c r="F3" s="136"/>
+      <c r="G3" s="136"/>
+      <c r="H3" s="136"/>
+      <c r="I3" s="137"/>
     </row>
     <row r="4" spans="1:9" ht="18.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A4" s="72" t="s">
         <v>44</v>
       </c>
-      <c r="B4" s="151" t="s">
+      <c r="B4" s="135" t="s">
         <v>167</v>
       </c>
-      <c r="C4" s="152"/>
-      <c r="D4" s="152"/>
-      <c r="E4" s="152"/>
-      <c r="F4" s="152"/>
-      <c r="G4" s="152"/>
-      <c r="H4" s="152"/>
-      <c r="I4" s="153"/>
+      <c r="C4" s="136"/>
+      <c r="D4" s="136"/>
+      <c r="E4" s="136"/>
+      <c r="F4" s="136"/>
+      <c r="G4" s="136"/>
+      <c r="H4" s="136"/>
+      <c r="I4" s="137"/>
     </row>
     <row r="5" spans="1:9" ht="26.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A5" s="72" t="s">
         <v>45</v>
       </c>
-      <c r="B5" s="151" t="s">
+      <c r="B5" s="135" t="s">
         <v>115</v>
       </c>
-      <c r="C5" s="152"/>
-      <c r="D5" s="152"/>
-      <c r="E5" s="152"/>
-      <c r="F5" s="152"/>
-      <c r="G5" s="152"/>
-      <c r="H5" s="152"/>
-      <c r="I5" s="153"/>
+      <c r="C5" s="136"/>
+      <c r="D5" s="136"/>
+      <c r="E5" s="136"/>
+      <c r="F5" s="136"/>
+      <c r="G5" s="136"/>
+      <c r="H5" s="136"/>
+      <c r="I5" s="137"/>
     </row>
     <row r="25" spans="2:10" ht="13.5" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="26" spans="2:10" ht="17.45" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B26" s="126" t="s">
+      <c r="B26" s="138" t="s">
         <v>169</v>
       </c>
-      <c r="C26" s="127"/>
-      <c r="D26" s="127"/>
-      <c r="E26" s="127"/>
-      <c r="F26" s="127"/>
-      <c r="G26" s="127"/>
-      <c r="H26" s="127"/>
-      <c r="I26" s="127"/>
-      <c r="J26" s="128"/>
+      <c r="C26" s="139"/>
+      <c r="D26" s="139"/>
+      <c r="E26" s="139"/>
+      <c r="F26" s="139"/>
+      <c r="G26" s="139"/>
+      <c r="H26" s="139"/>
+      <c r="I26" s="139"/>
+      <c r="J26" s="140"/>
     </row>
     <row r="27" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B27" s="129"/>
-      <c r="C27" s="130"/>
-      <c r="D27" s="130"/>
-      <c r="E27" s="130"/>
-      <c r="F27" s="130"/>
-      <c r="G27" s="130"/>
-      <c r="H27" s="130"/>
-      <c r="I27" s="130"/>
-      <c r="J27" s="131"/>
+      <c r="B27" s="141"/>
+      <c r="C27" s="142"/>
+      <c r="D27" s="142"/>
+      <c r="E27" s="142"/>
+      <c r="F27" s="142"/>
+      <c r="G27" s="142"/>
+      <c r="H27" s="142"/>
+      <c r="I27" s="142"/>
+      <c r="J27" s="143"/>
     </row>
     <row r="28" spans="2:10" ht="13.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B28" s="132"/>
-      <c r="C28" s="133"/>
-      <c r="D28" s="133"/>
-      <c r="E28" s="133"/>
-      <c r="F28" s="133"/>
-      <c r="G28" s="133"/>
-      <c r="H28" s="133"/>
-      <c r="I28" s="133"/>
-      <c r="J28" s="134"/>
+      <c r="B28" s="144"/>
+      <c r="C28" s="145"/>
+      <c r="D28" s="145"/>
+      <c r="E28" s="145"/>
+      <c r="F28" s="145"/>
+      <c r="G28" s="145"/>
+      <c r="H28" s="145"/>
+      <c r="I28" s="145"/>
+      <c r="J28" s="146"/>
     </row>
     <row r="29" spans="2:10" ht="13.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B29" s="60"/>
@@ -17413,17 +17520,17 @@
       <c r="I29" s="60"/>
     </row>
     <row r="30" spans="2:10" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B30" s="154" t="s">
+      <c r="B30" s="147" t="s">
         <v>166</v>
       </c>
-      <c r="C30" s="155"/>
-      <c r="D30" s="155"/>
-      <c r="E30" s="155"/>
-      <c r="F30" s="155"/>
-      <c r="G30" s="155"/>
-      <c r="H30" s="155"/>
-      <c r="I30" s="155"/>
-      <c r="J30" s="156"/>
+      <c r="C30" s="148"/>
+      <c r="D30" s="148"/>
+      <c r="E30" s="148"/>
+      <c r="F30" s="148"/>
+      <c r="G30" s="148"/>
+      <c r="H30" s="148"/>
+      <c r="I30" s="148"/>
+      <c r="J30" s="149"/>
     </row>
     <row r="31" spans="2:10" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B31" s="61"/>
@@ -17457,21 +17564,21 @@
       <c r="J33" s="61"/>
     </row>
     <row r="34" spans="2:10" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B34" s="144" t="s">
+      <c r="B34" s="128" t="s">
         <v>46</v>
       </c>
-      <c r="C34" s="145"/>
+      <c r="C34" s="129"/>
       <c r="D34" s="78" t="s">
         <v>47</v>
       </c>
-      <c r="E34" s="144" t="s">
+      <c r="E34" s="128" t="s">
         <v>106</v>
       </c>
-      <c r="F34" s="150"/>
-      <c r="G34" s="150"/>
-      <c r="H34" s="150"/>
-      <c r="I34" s="150"/>
-      <c r="J34" s="145"/>
+      <c r="F34" s="134"/>
+      <c r="G34" s="134"/>
+      <c r="H34" s="134"/>
+      <c r="I34" s="134"/>
+      <c r="J34" s="129"/>
     </row>
     <row r="35" spans="2:10" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B35" s="84" t="s">
@@ -17483,12 +17590,12 @@
       <c r="D35" s="84" t="s">
         <v>165</v>
       </c>
-      <c r="E35" s="160"/>
-      <c r="F35" s="160"/>
-      <c r="G35" s="160"/>
-      <c r="H35" s="160"/>
-      <c r="I35" s="160"/>
-      <c r="J35" s="160"/>
+      <c r="E35" s="161"/>
+      <c r="F35" s="161"/>
+      <c r="G35" s="161"/>
+      <c r="H35" s="161"/>
+      <c r="I35" s="161"/>
+      <c r="J35" s="161"/>
     </row>
     <row r="36" spans="2:10" ht="13.9" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B36" s="84" t="s">
@@ -17499,12 +17606,12 @@
         <v>0</v>
       </c>
       <c r="D36" s="87"/>
-      <c r="E36" s="160"/>
-      <c r="F36" s="160"/>
-      <c r="G36" s="160"/>
-      <c r="H36" s="160"/>
-      <c r="I36" s="160"/>
-      <c r="J36" s="160"/>
+      <c r="E36" s="161"/>
+      <c r="F36" s="161"/>
+      <c r="G36" s="161"/>
+      <c r="H36" s="161"/>
+      <c r="I36" s="161"/>
+      <c r="J36" s="161"/>
     </row>
     <row r="37" spans="2:10" ht="57" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B37" s="84" t="s">
@@ -17515,14 +17622,14 @@
         <v>0</v>
       </c>
       <c r="D37" s="88"/>
-      <c r="E37" s="161" t="s">
+      <c r="E37" s="159" t="s">
         <v>171</v>
       </c>
-      <c r="F37" s="162"/>
-      <c r="G37" s="162"/>
-      <c r="H37" s="162"/>
-      <c r="I37" s="162"/>
-      <c r="J37" s="162"/>
+      <c r="F37" s="160"/>
+      <c r="G37" s="160"/>
+      <c r="H37" s="160"/>
+      <c r="I37" s="160"/>
+      <c r="J37" s="160"/>
     </row>
     <row r="38" spans="2:10" ht="32.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B38" s="84" t="s">
@@ -17533,14 +17640,14 @@
         <v>0</v>
       </c>
       <c r="D38" s="88"/>
-      <c r="E38" s="161" t="s">
+      <c r="E38" s="159" t="s">
         <v>174</v>
       </c>
-      <c r="F38" s="162"/>
-      <c r="G38" s="162"/>
-      <c r="H38" s="162"/>
-      <c r="I38" s="162"/>
-      <c r="J38" s="162"/>
+      <c r="F38" s="160"/>
+      <c r="G38" s="160"/>
+      <c r="H38" s="160"/>
+      <c r="I38" s="160"/>
+      <c r="J38" s="160"/>
     </row>
     <row r="39" spans="2:10" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B39" s="84" t="s">
@@ -17553,14 +17660,14 @@
       <c r="D39" s="89" t="s">
         <v>28</v>
       </c>
-      <c r="E39" s="161" t="s">
+      <c r="E39" s="159" t="s">
         <v>109</v>
       </c>
-      <c r="F39" s="162"/>
-      <c r="G39" s="162"/>
-      <c r="H39" s="162"/>
-      <c r="I39" s="162"/>
-      <c r="J39" s="162"/>
+      <c r="F39" s="160"/>
+      <c r="G39" s="160"/>
+      <c r="H39" s="160"/>
+      <c r="I39" s="160"/>
+      <c r="J39" s="160"/>
     </row>
     <row r="40" spans="2:10" ht="36.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B40" s="84" t="s">
@@ -17573,14 +17680,14 @@
       <c r="D40" s="89" t="s">
         <v>29</v>
       </c>
-      <c r="E40" s="161" t="s">
+      <c r="E40" s="159" t="s">
         <v>173</v>
       </c>
-      <c r="F40" s="162"/>
-      <c r="G40" s="162"/>
-      <c r="H40" s="162"/>
-      <c r="I40" s="162"/>
-      <c r="J40" s="162"/>
+      <c r="F40" s="160"/>
+      <c r="G40" s="160"/>
+      <c r="H40" s="160"/>
+      <c r="I40" s="160"/>
+      <c r="J40" s="160"/>
     </row>
     <row r="41" spans="2:10" ht="27" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B41" s="84" t="s">
@@ -17593,14 +17700,14 @@
       <c r="D41" s="89" t="s">
         <v>31</v>
       </c>
-      <c r="E41" s="161" t="s">
+      <c r="E41" s="159" t="s">
         <v>172</v>
       </c>
-      <c r="F41" s="162"/>
-      <c r="G41" s="162"/>
-      <c r="H41" s="162"/>
-      <c r="I41" s="162"/>
-      <c r="J41" s="162"/>
+      <c r="F41" s="160"/>
+      <c r="G41" s="160"/>
+      <c r="H41" s="160"/>
+      <c r="I41" s="160"/>
+      <c r="J41" s="160"/>
     </row>
     <row r="42" spans="2:10" ht="55.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B42" s="84" t="s">
@@ -17613,14 +17720,14 @@
       <c r="D42" s="89" t="s">
         <v>30</v>
       </c>
-      <c r="E42" s="161" t="s">
+      <c r="E42" s="159" t="s">
         <v>175</v>
       </c>
-      <c r="F42" s="162"/>
-      <c r="G42" s="162"/>
-      <c r="H42" s="162"/>
-      <c r="I42" s="162"/>
-      <c r="J42" s="162"/>
+      <c r="F42" s="160"/>
+      <c r="G42" s="160"/>
+      <c r="H42" s="160"/>
+      <c r="I42" s="160"/>
+      <c r="J42" s="160"/>
     </row>
     <row r="43" spans="2:10" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B43" s="84" t="s">
@@ -17633,14 +17740,14 @@
       <c r="D43" s="89" t="s">
         <v>32</v>
       </c>
-      <c r="E43" s="161" t="s">
+      <c r="E43" s="159" t="s">
         <v>176</v>
       </c>
-      <c r="F43" s="162"/>
-      <c r="G43" s="162"/>
-      <c r="H43" s="162"/>
-      <c r="I43" s="162"/>
-      <c r="J43" s="162"/>
+      <c r="F43" s="160"/>
+      <c r="G43" s="160"/>
+      <c r="H43" s="160"/>
+      <c r="I43" s="160"/>
+      <c r="J43" s="160"/>
     </row>
     <row r="44" spans="2:10" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B44" s="84" t="s">
@@ -17652,14 +17759,14 @@
       <c r="D44" s="89" t="s">
         <v>40</v>
       </c>
-      <c r="E44" s="161" t="s">
+      <c r="E44" s="159" t="s">
         <v>120</v>
       </c>
-      <c r="F44" s="162"/>
-      <c r="G44" s="162"/>
-      <c r="H44" s="162"/>
-      <c r="I44" s="162"/>
-      <c r="J44" s="162"/>
+      <c r="F44" s="160"/>
+      <c r="G44" s="160"/>
+      <c r="H44" s="160"/>
+      <c r="I44" s="160"/>
+      <c r="J44" s="160"/>
     </row>
     <row r="45" spans="2:10" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B45" s="84" t="s">
@@ -17672,14 +17779,14 @@
       <c r="D45" s="89" t="s">
         <v>34</v>
       </c>
-      <c r="E45" s="160" t="s">
+      <c r="E45" s="161" t="s">
         <v>121</v>
       </c>
-      <c r="F45" s="160"/>
-      <c r="G45" s="160"/>
-      <c r="H45" s="160"/>
-      <c r="I45" s="160"/>
-      <c r="J45" s="160"/>
+      <c r="F45" s="161"/>
+      <c r="G45" s="161"/>
+      <c r="H45" s="161"/>
+      <c r="I45" s="161"/>
+      <c r="J45" s="161"/>
     </row>
     <row r="46" spans="2:10" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B46" s="84" t="s">
@@ -17691,14 +17798,14 @@
       <c r="D46" s="89" t="s">
         <v>35</v>
       </c>
-      <c r="E46" s="160" t="s">
+      <c r="E46" s="161" t="s">
         <v>121</v>
       </c>
-      <c r="F46" s="160"/>
-      <c r="G46" s="160"/>
-      <c r="H46" s="160"/>
-      <c r="I46" s="160"/>
-      <c r="J46" s="160"/>
+      <c r="F46" s="161"/>
+      <c r="G46" s="161"/>
+      <c r="H46" s="161"/>
+      <c r="I46" s="161"/>
+      <c r="J46" s="161"/>
     </row>
     <row r="47" spans="2:10" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B47" s="84" t="s">
@@ -17710,14 +17817,14 @@
       <c r="D47" s="89" t="s">
         <v>41</v>
       </c>
-      <c r="E47" s="160" t="s">
+      <c r="E47" s="161" t="s">
         <v>121</v>
       </c>
-      <c r="F47" s="160"/>
-      <c r="G47" s="160"/>
-      <c r="H47" s="160"/>
-      <c r="I47" s="160"/>
-      <c r="J47" s="160"/>
+      <c r="F47" s="161"/>
+      <c r="G47" s="161"/>
+      <c r="H47" s="161"/>
+      <c r="I47" s="161"/>
+      <c r="J47" s="161"/>
     </row>
     <row r="48" spans="2:10" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B48" s="84" t="s">
@@ -17730,58 +17837,58 @@
       <c r="D48" s="89" t="s">
         <v>42</v>
       </c>
-      <c r="E48" s="160"/>
-      <c r="F48" s="160"/>
-      <c r="G48" s="160"/>
-      <c r="H48" s="160"/>
-      <c r="I48" s="160"/>
-      <c r="J48" s="160"/>
+      <c r="E48" s="161"/>
+      <c r="F48" s="161"/>
+      <c r="G48" s="161"/>
+      <c r="H48" s="161"/>
+      <c r="I48" s="161"/>
+      <c r="J48" s="161"/>
     </row>
     <row r="49" spans="2:10" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B49" s="83"/>
       <c r="C49" s="83"/>
       <c r="D49" s="83"/>
-      <c r="E49" s="157"/>
-      <c r="F49" s="158"/>
-      <c r="G49" s="158"/>
-      <c r="H49" s="158"/>
-      <c r="I49" s="158"/>
-      <c r="J49" s="159"/>
+      <c r="E49" s="162"/>
+      <c r="F49" s="163"/>
+      <c r="G49" s="163"/>
+      <c r="H49" s="163"/>
+      <c r="I49" s="163"/>
+      <c r="J49" s="164"/>
     </row>
     <row r="50" spans="2:10" ht="17.45" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B50" s="126" t="s">
+      <c r="B50" s="138" t="s">
         <v>170</v>
       </c>
-      <c r="C50" s="127"/>
-      <c r="D50" s="127"/>
-      <c r="E50" s="127"/>
-      <c r="F50" s="127"/>
-      <c r="G50" s="127"/>
-      <c r="H50" s="127"/>
-      <c r="I50" s="127"/>
-      <c r="J50" s="128"/>
+      <c r="C50" s="139"/>
+      <c r="D50" s="139"/>
+      <c r="E50" s="139"/>
+      <c r="F50" s="139"/>
+      <c r="G50" s="139"/>
+      <c r="H50" s="139"/>
+      <c r="I50" s="139"/>
+      <c r="J50" s="140"/>
     </row>
     <row r="51" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B51" s="129"/>
-      <c r="C51" s="130"/>
-      <c r="D51" s="130"/>
-      <c r="E51" s="130"/>
-      <c r="F51" s="130"/>
-      <c r="G51" s="130"/>
-      <c r="H51" s="130"/>
-      <c r="I51" s="130"/>
-      <c r="J51" s="131"/>
+      <c r="B51" s="141"/>
+      <c r="C51" s="142"/>
+      <c r="D51" s="142"/>
+      <c r="E51" s="142"/>
+      <c r="F51" s="142"/>
+      <c r="G51" s="142"/>
+      <c r="H51" s="142"/>
+      <c r="I51" s="142"/>
+      <c r="J51" s="143"/>
     </row>
     <row r="52" spans="2:10" ht="13.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B52" s="132"/>
-      <c r="C52" s="133"/>
-      <c r="D52" s="133"/>
-      <c r="E52" s="133"/>
-      <c r="F52" s="133"/>
-      <c r="G52" s="133"/>
-      <c r="H52" s="133"/>
-      <c r="I52" s="133"/>
-      <c r="J52" s="134"/>
+      <c r="B52" s="144"/>
+      <c r="C52" s="145"/>
+      <c r="D52" s="145"/>
+      <c r="E52" s="145"/>
+      <c r="F52" s="145"/>
+      <c r="G52" s="145"/>
+      <c r="H52" s="145"/>
+      <c r="I52" s="145"/>
+      <c r="J52" s="146"/>
     </row>
     <row r="53" spans="2:10" ht="13.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B53" s="61"/>
@@ -17830,12 +17937,17 @@
     </row>
   </sheetData>
   <mergeCells count="24">
-    <mergeCell ref="B30:J30"/>
-    <mergeCell ref="A2:I2"/>
-    <mergeCell ref="B3:I3"/>
-    <mergeCell ref="B4:I4"/>
-    <mergeCell ref="B5:I5"/>
-    <mergeCell ref="B26:J28"/>
+    <mergeCell ref="E49:J49"/>
+    <mergeCell ref="B50:J52"/>
+    <mergeCell ref="E46:J46"/>
+    <mergeCell ref="E47:J47"/>
+    <mergeCell ref="E48:J48"/>
+    <mergeCell ref="E43:J43"/>
+    <mergeCell ref="E44:J44"/>
+    <mergeCell ref="E45:J45"/>
+    <mergeCell ref="E40:J40"/>
+    <mergeCell ref="E41:J41"/>
+    <mergeCell ref="E42:J42"/>
     <mergeCell ref="E37:J37"/>
     <mergeCell ref="E38:J38"/>
     <mergeCell ref="E39:J39"/>
@@ -17843,17 +17955,12 @@
     <mergeCell ref="E34:J34"/>
     <mergeCell ref="E35:J35"/>
     <mergeCell ref="E36:J36"/>
-    <mergeCell ref="E43:J43"/>
-    <mergeCell ref="E44:J44"/>
-    <mergeCell ref="E45:J45"/>
-    <mergeCell ref="E40:J40"/>
-    <mergeCell ref="E41:J41"/>
-    <mergeCell ref="E42:J42"/>
-    <mergeCell ref="E49:J49"/>
-    <mergeCell ref="B50:J52"/>
-    <mergeCell ref="E46:J46"/>
-    <mergeCell ref="E47:J47"/>
-    <mergeCell ref="E48:J48"/>
+    <mergeCell ref="B30:J30"/>
+    <mergeCell ref="A2:I2"/>
+    <mergeCell ref="B3:I3"/>
+    <mergeCell ref="B4:I4"/>
+    <mergeCell ref="B5:I5"/>
+    <mergeCell ref="B26:J28"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>

</xml_diff>